<commit_message>
first run of Vlookup
</commit_message>
<xml_diff>
--- a/transformation_workbook.xlsx
+++ b/transformation_workbook.xlsx
@@ -476,7 +476,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13.5" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
@@ -2788,7 +2788,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13.5" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
@@ -3558,7 +3558,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13.5" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
@@ -4360,7 +4360,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13.5" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
@@ -5929,7 +5929,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13.5" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
@@ -6492,7 +6492,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13.5" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
@@ -7062,7 +7062,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13.5" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="7.33203125" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -7626,7 +7626,7 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13.5" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
@@ -8382,7 +8382,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13.5" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="5" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -10946,6 +10946,21 @@
           <t>Detroit</t>
         </is>
       </c>
+      <c r="B2" t="n">
+        <v>27.4</v>
+      </c>
+      <c r="C2" t="n">
+        <v>36.3</v>
+      </c>
+      <c r="D2" t="n">
+        <v>47</v>
+      </c>
+      <c r="E2" t="n">
+        <v>28</v>
+      </c>
+      <c r="F2" t="n">
+        <v>33.5</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -10953,6 +10968,21 @@
           <t>Washington</t>
         </is>
       </c>
+      <c r="B3" t="n">
+        <v>19.4</v>
+      </c>
+      <c r="C3" t="n">
+        <v>33</v>
+      </c>
+      <c r="D3" t="n">
+        <v>23</v>
+      </c>
+      <c r="E3" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="F3" t="n">
+        <v>30.8</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -10960,6 +10990,21 @@
           <t>Tampa Bay</t>
         </is>
       </c>
+      <c r="B4" t="n">
+        <v>21.2</v>
+      </c>
+      <c r="C4" t="n">
+        <v>38</v>
+      </c>
+      <c r="D4" t="n">
+        <v>51</v>
+      </c>
+      <c r="E4" t="n">
+        <v>25.7</v>
+      </c>
+      <c r="F4" t="n">
+        <v>33.7</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -10967,6 +11012,21 @@
           <t>Baltimore</t>
         </is>
       </c>
+      <c r="B5" t="n">
+        <v>27.7</v>
+      </c>
+      <c r="C5" t="n">
+        <v>35.3</v>
+      </c>
+      <c r="D5" t="n">
+        <v>30</v>
+      </c>
+      <c r="E5" t="n">
+        <v>29.3</v>
+      </c>
+      <c r="F5" t="n">
+        <v>29.7</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -10974,6 +11034,21 @@
           <t>Minnesota</t>
         </is>
       </c>
+      <c r="B6" t="n">
+        <v>20.2</v>
+      </c>
+      <c r="C6" t="n">
+        <v>29.3</v>
+      </c>
+      <c r="D6" t="n">
+        <v>23</v>
+      </c>
+      <c r="E6" t="n">
+        <v>28.5</v>
+      </c>
+      <c r="F6" t="n">
+        <v>27.3</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -10981,6 +11056,21 @@
           <t>Buffalo</t>
         </is>
       </c>
+      <c r="B7" t="n">
+        <v>26.6</v>
+      </c>
+      <c r="C7" t="n">
+        <v>17.7</v>
+      </c>
+      <c r="D7" t="n">
+        <v>23</v>
+      </c>
+      <c r="E7" t="n">
+        <v>40.5</v>
+      </c>
+      <c r="F7" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -10988,6 +11078,21 @@
           <t>San Francisco</t>
         </is>
       </c>
+      <c r="B8" t="n">
+        <v>28.6</v>
+      </c>
+      <c r="C8" t="n">
+        <v>29.7</v>
+      </c>
+      <c r="D8" t="n">
+        <v>36</v>
+      </c>
+      <c r="E8" t="n">
+        <v>28.3</v>
+      </c>
+      <c r="F8" t="n">
+        <v>25.7</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -10995,6 +11100,21 @@
           <t>Green Bay</t>
         </is>
       </c>
+      <c r="B9" t="n">
+        <v>23.8</v>
+      </c>
+      <c r="C9" t="n">
+        <v>29</v>
+      </c>
+      <c r="D9" t="n">
+        <v>34</v>
+      </c>
+      <c r="E9" t="n">
+        <v>26.3</v>
+      </c>
+      <c r="F9" t="n">
+        <v>27.7</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -11002,6 +11122,21 @@
           <t>Cincinnati</t>
         </is>
       </c>
+      <c r="B10" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="C10" t="n">
+        <v>29.7</v>
+      </c>
+      <c r="D10" t="n">
+        <v>17</v>
+      </c>
+      <c r="E10" t="n">
+        <v>27</v>
+      </c>
+      <c r="F10" t="n">
+        <v>25.3</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -11009,6 +11144,21 @@
           <t>New Orleans</t>
         </is>
       </c>
+      <c r="B11" t="n">
+        <v>23.6</v>
+      </c>
+      <c r="C11" t="n">
+        <v>16.7</v>
+      </c>
+      <c r="D11" t="n">
+        <v>10</v>
+      </c>
+      <c r="E11" t="n">
+        <v>24</v>
+      </c>
+      <c r="F11" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -11016,6 +11166,21 @@
           <t>Atlanta</t>
         </is>
       </c>
+      <c r="B12" t="n">
+        <v>18.9</v>
+      </c>
+      <c r="C12" t="n">
+        <v>33.3</v>
+      </c>
+      <c r="D12" t="n">
+        <v>38</v>
+      </c>
+      <c r="E12" t="n">
+        <v>22.3</v>
+      </c>
+      <c r="F12" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -11023,6 +11188,21 @@
           <t>Chicago</t>
         </is>
       </c>
+      <c r="B13" t="n">
+        <v>21.2</v>
+      </c>
+      <c r="C13" t="n">
+        <v>31.7</v>
+      </c>
+      <c r="D13" t="n">
+        <v>35</v>
+      </c>
+      <c r="E13" t="n">
+        <v>28</v>
+      </c>
+      <c r="F13" t="n">
+        <v>21.3</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -11030,6 +11210,21 @@
           <t>Seattle</t>
         </is>
       </c>
+      <c r="B14" t="n">
+        <v>21.4</v>
+      </c>
+      <c r="C14" t="n">
+        <v>24.3</v>
+      </c>
+      <c r="D14" t="n">
+        <v>24</v>
+      </c>
+      <c r="E14" t="n">
+        <v>23.5</v>
+      </c>
+      <c r="F14" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -11037,6 +11232,21 @@
           <t>Houston</t>
         </is>
       </c>
+      <c r="B15" t="n">
+        <v>22.7</v>
+      </c>
+      <c r="C15" t="n">
+        <v>29.3</v>
+      </c>
+      <c r="D15" t="n">
+        <v>41</v>
+      </c>
+      <c r="E15" t="n">
+        <v>22</v>
+      </c>
+      <c r="F15" t="n">
+        <v>25.7</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -11044,6 +11254,21 @@
           <t>Kansas City</t>
         </is>
       </c>
+      <c r="B16" t="n">
+        <v>22.2</v>
+      </c>
+      <c r="C16" t="n">
+        <v>21.7</v>
+      </c>
+      <c r="D16" t="n">
+        <v>26</v>
+      </c>
+      <c r="E16" t="n">
+        <v>26.3</v>
+      </c>
+      <c r="F16" t="n">
+        <v>19.5</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -11051,6 +11276,21 @@
           <t>Indianapolis</t>
         </is>
       </c>
+      <c r="B17" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="C17" t="n">
+        <v>27</v>
+      </c>
+      <c r="D17" t="n">
+        <v>20</v>
+      </c>
+      <c r="E17" t="n">
+        <v>25</v>
+      </c>
+      <c r="F17" t="n">
+        <v>21.3</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -11058,6 +11298,21 @@
           <t>Arizona</t>
         </is>
       </c>
+      <c r="B18" t="n">
+        <v>19.4</v>
+      </c>
+      <c r="C18" t="n">
+        <v>17</v>
+      </c>
+      <c r="D18" t="n">
+        <v>13</v>
+      </c>
+      <c r="E18" t="n">
+        <v>22.7</v>
+      </c>
+      <c r="F18" t="n">
+        <v>21.7</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -11065,6 +11320,21 @@
           <t>Philadelphia</t>
         </is>
       </c>
+      <c r="B19" t="n">
+        <v>24.6</v>
+      </c>
+      <c r="C19" t="n">
+        <v>17</v>
+      </c>
+      <c r="D19" t="n">
+        <v>20</v>
+      </c>
+      <c r="E19" t="n">
+        <v>20.5</v>
+      </c>
+      <c r="F19" t="n">
+        <v>21.7</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -11072,6 +11342,21 @@
           <t>Dallas</t>
         </is>
       </c>
+      <c r="B20" t="n">
+        <v>30.1</v>
+      </c>
+      <c r="C20" t="n">
+        <v>16.3</v>
+      </c>
+      <c r="D20" t="n">
+        <v>9</v>
+      </c>
+      <c r="E20" t="n">
+        <v>17.7</v>
+      </c>
+      <c r="F20" t="n">
+        <v>24.3</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -11079,6 +11364,21 @@
           <t>Denver</t>
         </is>
       </c>
+      <c r="B21" t="n">
+        <v>21</v>
+      </c>
+      <c r="C21" t="n">
+        <v>27.7</v>
+      </c>
+      <c r="D21" t="n">
+        <v>33</v>
+      </c>
+      <c r="E21" t="n">
+        <v>18.7</v>
+      </c>
+      <c r="F21" t="n">
+        <v>22.3</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -11086,6 +11386,21 @@
           <t>Pittsburgh</t>
         </is>
       </c>
+      <c r="B22" t="n">
+        <v>17.8</v>
+      </c>
+      <c r="C22" t="n">
+        <v>24.3</v>
+      </c>
+      <c r="D22" t="n">
+        <v>32</v>
+      </c>
+      <c r="E22" t="n">
+        <v>18.5</v>
+      </c>
+      <c r="F22" t="n">
+        <v>21.8</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -11093,6 +11408,21 @@
           <t>Tennessee</t>
         </is>
       </c>
+      <c r="B23" t="n">
+        <v>17.9</v>
+      </c>
+      <c r="C23" t="n">
+        <v>20.7</v>
+      </c>
+      <c r="D23" t="n">
+        <v>17</v>
+      </c>
+      <c r="E23" t="n">
+        <v>16</v>
+      </c>
+      <c r="F23" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -11100,6 +11430,21 @@
           <t>Jacksonville</t>
         </is>
       </c>
+      <c r="B24" t="n">
+        <v>22.2</v>
+      </c>
+      <c r="C24" t="n">
+        <v>24.3</v>
+      </c>
+      <c r="D24" t="n">
+        <v>16</v>
+      </c>
+      <c r="E24" t="n">
+        <v>25</v>
+      </c>
+      <c r="F24" t="n">
+        <v>15.8</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -11107,6 +11452,21 @@
           <t>NY Jets</t>
         </is>
       </c>
+      <c r="B25" t="n">
+        <v>15.8</v>
+      </c>
+      <c r="C25" t="n">
+        <v>15.3</v>
+      </c>
+      <c r="D25" t="n">
+        <v>20</v>
+      </c>
+      <c r="E25" t="n">
+        <v>17.7</v>
+      </c>
+      <c r="F25" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -11114,6 +11474,21 @@
           <t>LA Rams</t>
         </is>
       </c>
+      <c r="B26" t="n">
+        <v>23.7</v>
+      </c>
+      <c r="C26" t="n">
+        <v>21.3</v>
+      </c>
+      <c r="D26" t="n">
+        <v>19</v>
+      </c>
+      <c r="E26" t="n">
+        <v>23</v>
+      </c>
+      <c r="F26" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -11121,6 +11496,21 @@
           <t>LA Chargers</t>
         </is>
       </c>
+      <c r="B27" t="n">
+        <v>20.4</v>
+      </c>
+      <c r="C27" t="n">
+        <v>14.3</v>
+      </c>
+      <c r="D27" t="n">
+        <v>23</v>
+      </c>
+      <c r="E27" t="n">
+        <v>16</v>
+      </c>
+      <c r="F27" t="n">
+        <v>19.7</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -11128,6 +11518,21 @@
           <t>Las Vegas</t>
         </is>
       </c>
+      <c r="B28" t="n">
+        <v>19.5</v>
+      </c>
+      <c r="C28" t="n">
+        <v>17</v>
+      </c>
+      <c r="D28" t="n">
+        <v>13</v>
+      </c>
+      <c r="E28" t="n">
+        <v>18.3</v>
+      </c>
+      <c r="F28" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -11135,6 +11540,21 @@
           <t>Carolina</t>
         </is>
       </c>
+      <c r="B29" t="n">
+        <v>13.9</v>
+      </c>
+      <c r="C29" t="n">
+        <v>18</v>
+      </c>
+      <c r="D29" t="n">
+        <v>20</v>
+      </c>
+      <c r="E29" t="n">
+        <v>15.7</v>
+      </c>
+      <c r="F29" t="n">
+        <v>18.7</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -11142,6 +11562,21 @@
           <t>NY Giants</t>
         </is>
       </c>
+      <c r="B30" t="n">
+        <v>15.6</v>
+      </c>
+      <c r="C30" t="n">
+        <v>17</v>
+      </c>
+      <c r="D30" t="n">
+        <v>7</v>
+      </c>
+      <c r="E30" t="n">
+        <v>9.300000000000001</v>
+      </c>
+      <c r="F30" t="n">
+        <v>22.7</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -11149,6 +11584,21 @@
           <t>Cleveland</t>
         </is>
       </c>
+      <c r="B31" t="n">
+        <v>22.8</v>
+      </c>
+      <c r="C31" t="n">
+        <v>15</v>
+      </c>
+      <c r="D31" t="n">
+        <v>16</v>
+      </c>
+      <c r="E31" t="n">
+        <v>16</v>
+      </c>
+      <c r="F31" t="n">
+        <v>15.8</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -11156,12 +11606,42 @@
           <t>New England</t>
         </is>
       </c>
+      <c r="B32" t="n">
+        <v>13.9</v>
+      </c>
+      <c r="C32" t="n">
+        <v>14.7</v>
+      </c>
+      <c r="D32" t="n">
+        <v>21</v>
+      </c>
+      <c r="E32" t="n">
+        <v>17</v>
+      </c>
+      <c r="F32" t="n">
+        <v>10.7</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
           <t>Miami</t>
         </is>
+      </c>
+      <c r="B33" t="n">
+        <v>27.9</v>
+      </c>
+      <c r="C33" t="n">
+        <v>10</v>
+      </c>
+      <c r="D33" t="n">
+        <v>15</v>
+      </c>
+      <c r="E33" t="n">
+        <v>14</v>
+      </c>
+      <c r="F33" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -11181,7 +11661,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13.5" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
@@ -12825,7 +13305,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13.33203125" customWidth="1" min="1" max="1"/>
   </cols>

</xml_diff>

<commit_message>
fixing code to start new vlookup
</commit_message>
<xml_diff>
--- a/transformation_workbook.xlsx
+++ b/transformation_workbook.xlsx
@@ -476,7 +476,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col width="13.5" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
@@ -2788,7 +2788,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col width="13.5" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
@@ -3558,7 +3558,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col width="13.5" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
@@ -4360,7 +4360,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col width="13.5" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
@@ -5929,7 +5929,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col width="13.5" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
@@ -6492,7 +6492,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col width="13.5" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
@@ -7062,7 +7062,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col width="13.5" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="7.33203125" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -7626,7 +7626,7 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col width="13.5" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
@@ -8382,7 +8382,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col width="13.5" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="5" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -10946,21 +10946,6 @@
           <t>Detroit</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>27.4</v>
-      </c>
-      <c r="C2" t="n">
-        <v>36.3</v>
-      </c>
-      <c r="D2" t="n">
-        <v>47</v>
-      </c>
-      <c r="E2" t="n">
-        <v>28</v>
-      </c>
-      <c r="F2" t="n">
-        <v>33.5</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -10968,21 +10953,6 @@
           <t>Washington</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>19.4</v>
-      </c>
-      <c r="C3" t="n">
-        <v>33</v>
-      </c>
-      <c r="D3" t="n">
-        <v>23</v>
-      </c>
-      <c r="E3" t="n">
-        <v>27.5</v>
-      </c>
-      <c r="F3" t="n">
-        <v>30.8</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -10990,21 +10960,6 @@
           <t>Tampa Bay</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>21.2</v>
-      </c>
-      <c r="C4" t="n">
-        <v>38</v>
-      </c>
-      <c r="D4" t="n">
-        <v>51</v>
-      </c>
-      <c r="E4" t="n">
-        <v>25.7</v>
-      </c>
-      <c r="F4" t="n">
-        <v>33.7</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -11012,21 +10967,6 @@
           <t>Baltimore</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>27.7</v>
-      </c>
-      <c r="C5" t="n">
-        <v>35.3</v>
-      </c>
-      <c r="D5" t="n">
-        <v>30</v>
-      </c>
-      <c r="E5" t="n">
-        <v>29.3</v>
-      </c>
-      <c r="F5" t="n">
-        <v>29.7</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -11034,21 +10974,6 @@
           <t>Minnesota</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>20.2</v>
-      </c>
-      <c r="C6" t="n">
-        <v>29.3</v>
-      </c>
-      <c r="D6" t="n">
-        <v>23</v>
-      </c>
-      <c r="E6" t="n">
-        <v>28.5</v>
-      </c>
-      <c r="F6" t="n">
-        <v>27.3</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -11056,21 +10981,6 @@
           <t>Buffalo</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>26.6</v>
-      </c>
-      <c r="C7" t="n">
-        <v>17.7</v>
-      </c>
-      <c r="D7" t="n">
-        <v>23</v>
-      </c>
-      <c r="E7" t="n">
-        <v>40.5</v>
-      </c>
-      <c r="F7" t="n">
-        <v>21</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -11078,21 +10988,6 @@
           <t>San Francisco</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>28.6</v>
-      </c>
-      <c r="C8" t="n">
-        <v>29.7</v>
-      </c>
-      <c r="D8" t="n">
-        <v>36</v>
-      </c>
-      <c r="E8" t="n">
-        <v>28.3</v>
-      </c>
-      <c r="F8" t="n">
-        <v>25.7</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -11100,21 +10995,6 @@
           <t>Green Bay</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>23.8</v>
-      </c>
-      <c r="C9" t="n">
-        <v>29</v>
-      </c>
-      <c r="D9" t="n">
-        <v>34</v>
-      </c>
-      <c r="E9" t="n">
-        <v>26.3</v>
-      </c>
-      <c r="F9" t="n">
-        <v>27.7</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -11122,21 +11002,6 @@
           <t>Cincinnati</t>
         </is>
       </c>
-      <c r="B10" t="n">
-        <v>21.5</v>
-      </c>
-      <c r="C10" t="n">
-        <v>29.7</v>
-      </c>
-      <c r="D10" t="n">
-        <v>17</v>
-      </c>
-      <c r="E10" t="n">
-        <v>27</v>
-      </c>
-      <c r="F10" t="n">
-        <v>25.3</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -11144,21 +11009,6 @@
           <t>New Orleans</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>23.6</v>
-      </c>
-      <c r="C11" t="n">
-        <v>16.7</v>
-      </c>
-      <c r="D11" t="n">
-        <v>10</v>
-      </c>
-      <c r="E11" t="n">
-        <v>24</v>
-      </c>
-      <c r="F11" t="n">
-        <v>27</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -11166,21 +11016,6 @@
           <t>Atlanta</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>18.9</v>
-      </c>
-      <c r="C12" t="n">
-        <v>33.3</v>
-      </c>
-      <c r="D12" t="n">
-        <v>38</v>
-      </c>
-      <c r="E12" t="n">
-        <v>22.3</v>
-      </c>
-      <c r="F12" t="n">
-        <v>30</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -11188,21 +11023,6 @@
           <t>Chicago</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>21.2</v>
-      </c>
-      <c r="C13" t="n">
-        <v>31.7</v>
-      </c>
-      <c r="D13" t="n">
-        <v>35</v>
-      </c>
-      <c r="E13" t="n">
-        <v>28</v>
-      </c>
-      <c r="F13" t="n">
-        <v>21.3</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -11210,21 +11030,6 @@
           <t>Seattle</t>
         </is>
       </c>
-      <c r="B14" t="n">
-        <v>21.4</v>
-      </c>
-      <c r="C14" t="n">
-        <v>24.3</v>
-      </c>
-      <c r="D14" t="n">
-        <v>24</v>
-      </c>
-      <c r="E14" t="n">
-        <v>23.5</v>
-      </c>
-      <c r="F14" t="n">
-        <v>26</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -11232,21 +11037,6 @@
           <t>Houston</t>
         </is>
       </c>
-      <c r="B15" t="n">
-        <v>22.7</v>
-      </c>
-      <c r="C15" t="n">
-        <v>29.3</v>
-      </c>
-      <c r="D15" t="n">
-        <v>41</v>
-      </c>
-      <c r="E15" t="n">
-        <v>22</v>
-      </c>
-      <c r="F15" t="n">
-        <v>25.7</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -11254,21 +11044,6 @@
           <t>Kansas City</t>
         </is>
       </c>
-      <c r="B16" t="n">
-        <v>22.2</v>
-      </c>
-      <c r="C16" t="n">
-        <v>21.7</v>
-      </c>
-      <c r="D16" t="n">
-        <v>26</v>
-      </c>
-      <c r="E16" t="n">
-        <v>26.3</v>
-      </c>
-      <c r="F16" t="n">
-        <v>19.5</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -11276,21 +11051,6 @@
           <t>Indianapolis</t>
         </is>
       </c>
-      <c r="B17" t="n">
-        <v>23.3</v>
-      </c>
-      <c r="C17" t="n">
-        <v>27</v>
-      </c>
-      <c r="D17" t="n">
-        <v>20</v>
-      </c>
-      <c r="E17" t="n">
-        <v>25</v>
-      </c>
-      <c r="F17" t="n">
-        <v>21.3</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -11298,21 +11058,6 @@
           <t>Arizona</t>
         </is>
       </c>
-      <c r="B18" t="n">
-        <v>19.4</v>
-      </c>
-      <c r="C18" t="n">
-        <v>17</v>
-      </c>
-      <c r="D18" t="n">
-        <v>13</v>
-      </c>
-      <c r="E18" t="n">
-        <v>22.7</v>
-      </c>
-      <c r="F18" t="n">
-        <v>21.7</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -11320,21 +11065,6 @@
           <t>Philadelphia</t>
         </is>
       </c>
-      <c r="B19" t="n">
-        <v>24.6</v>
-      </c>
-      <c r="C19" t="n">
-        <v>17</v>
-      </c>
-      <c r="D19" t="n">
-        <v>20</v>
-      </c>
-      <c r="E19" t="n">
-        <v>20.5</v>
-      </c>
-      <c r="F19" t="n">
-        <v>21.7</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -11342,21 +11072,6 @@
           <t>Dallas</t>
         </is>
       </c>
-      <c r="B20" t="n">
-        <v>30.1</v>
-      </c>
-      <c r="C20" t="n">
-        <v>16.3</v>
-      </c>
-      <c r="D20" t="n">
-        <v>9</v>
-      </c>
-      <c r="E20" t="n">
-        <v>17.7</v>
-      </c>
-      <c r="F20" t="n">
-        <v>24.3</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -11364,21 +11079,6 @@
           <t>Denver</t>
         </is>
       </c>
-      <c r="B21" t="n">
-        <v>21</v>
-      </c>
-      <c r="C21" t="n">
-        <v>27.7</v>
-      </c>
-      <c r="D21" t="n">
-        <v>33</v>
-      </c>
-      <c r="E21" t="n">
-        <v>18.7</v>
-      </c>
-      <c r="F21" t="n">
-        <v>22.3</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -11386,21 +11086,6 @@
           <t>Pittsburgh</t>
         </is>
       </c>
-      <c r="B22" t="n">
-        <v>17.8</v>
-      </c>
-      <c r="C22" t="n">
-        <v>24.3</v>
-      </c>
-      <c r="D22" t="n">
-        <v>32</v>
-      </c>
-      <c r="E22" t="n">
-        <v>18.5</v>
-      </c>
-      <c r="F22" t="n">
-        <v>21.8</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -11408,21 +11093,6 @@
           <t>Tennessee</t>
         </is>
       </c>
-      <c r="B23" t="n">
-        <v>17.9</v>
-      </c>
-      <c r="C23" t="n">
-        <v>20.7</v>
-      </c>
-      <c r="D23" t="n">
-        <v>17</v>
-      </c>
-      <c r="E23" t="n">
-        <v>16</v>
-      </c>
-      <c r="F23" t="n">
-        <v>24</v>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -11430,21 +11100,6 @@
           <t>Jacksonville</t>
         </is>
       </c>
-      <c r="B24" t="n">
-        <v>22.2</v>
-      </c>
-      <c r="C24" t="n">
-        <v>24.3</v>
-      </c>
-      <c r="D24" t="n">
-        <v>16</v>
-      </c>
-      <c r="E24" t="n">
-        <v>25</v>
-      </c>
-      <c r="F24" t="n">
-        <v>15.8</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -11452,21 +11107,6 @@
           <t>NY Jets</t>
         </is>
       </c>
-      <c r="B25" t="n">
-        <v>15.8</v>
-      </c>
-      <c r="C25" t="n">
-        <v>15.3</v>
-      </c>
-      <c r="D25" t="n">
-        <v>20</v>
-      </c>
-      <c r="E25" t="n">
-        <v>17.7</v>
-      </c>
-      <c r="F25" t="n">
-        <v>20</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -11474,21 +11114,6 @@
           <t>LA Rams</t>
         </is>
       </c>
-      <c r="B26" t="n">
-        <v>23.7</v>
-      </c>
-      <c r="C26" t="n">
-        <v>21.3</v>
-      </c>
-      <c r="D26" t="n">
-        <v>19</v>
-      </c>
-      <c r="E26" t="n">
-        <v>23</v>
-      </c>
-      <c r="F26" t="n">
-        <v>16</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -11496,21 +11121,6 @@
           <t>LA Chargers</t>
         </is>
       </c>
-      <c r="B27" t="n">
-        <v>20.4</v>
-      </c>
-      <c r="C27" t="n">
-        <v>14.3</v>
-      </c>
-      <c r="D27" t="n">
-        <v>23</v>
-      </c>
-      <c r="E27" t="n">
-        <v>16</v>
-      </c>
-      <c r="F27" t="n">
-        <v>19.7</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -11518,21 +11128,6 @@
           <t>Las Vegas</t>
         </is>
       </c>
-      <c r="B28" t="n">
-        <v>19.5</v>
-      </c>
-      <c r="C28" t="n">
-        <v>17</v>
-      </c>
-      <c r="D28" t="n">
-        <v>13</v>
-      </c>
-      <c r="E28" t="n">
-        <v>18.3</v>
-      </c>
-      <c r="F28" t="n">
-        <v>18</v>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -11540,21 +11135,6 @@
           <t>Carolina</t>
         </is>
       </c>
-      <c r="B29" t="n">
-        <v>13.9</v>
-      </c>
-      <c r="C29" t="n">
-        <v>18</v>
-      </c>
-      <c r="D29" t="n">
-        <v>20</v>
-      </c>
-      <c r="E29" t="n">
-        <v>15.7</v>
-      </c>
-      <c r="F29" t="n">
-        <v>18.7</v>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -11562,21 +11142,6 @@
           <t>NY Giants</t>
         </is>
       </c>
-      <c r="B30" t="n">
-        <v>15.6</v>
-      </c>
-      <c r="C30" t="n">
-        <v>17</v>
-      </c>
-      <c r="D30" t="n">
-        <v>7</v>
-      </c>
-      <c r="E30" t="n">
-        <v>9.300000000000001</v>
-      </c>
-      <c r="F30" t="n">
-        <v>22.7</v>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -11584,21 +11149,6 @@
           <t>Cleveland</t>
         </is>
       </c>
-      <c r="B31" t="n">
-        <v>22.8</v>
-      </c>
-      <c r="C31" t="n">
-        <v>15</v>
-      </c>
-      <c r="D31" t="n">
-        <v>16</v>
-      </c>
-      <c r="E31" t="n">
-        <v>16</v>
-      </c>
-      <c r="F31" t="n">
-        <v>15.8</v>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -11606,42 +11156,12 @@
           <t>New England</t>
         </is>
       </c>
-      <c r="B32" t="n">
-        <v>13.9</v>
-      </c>
-      <c r="C32" t="n">
-        <v>14.7</v>
-      </c>
-      <c r="D32" t="n">
-        <v>21</v>
-      </c>
-      <c r="E32" t="n">
-        <v>17</v>
-      </c>
-      <c r="F32" t="n">
-        <v>10.7</v>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
           <t>Miami</t>
         </is>
-      </c>
-      <c r="B33" t="n">
-        <v>27.9</v>
-      </c>
-      <c r="C33" t="n">
-        <v>10</v>
-      </c>
-      <c r="D33" t="n">
-        <v>15</v>
-      </c>
-      <c r="E33" t="n">
-        <v>14</v>
-      </c>
-      <c r="F33" t="n">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -11661,7 +11181,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col width="13.5" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
@@ -13305,7 +12825,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col width="13.33203125" customWidth="1" min="1" max="1"/>
   </cols>

</xml_diff>

<commit_message>
created a working vlookup function
</commit_message>
<xml_diff>
--- a/transformation_workbook.xlsx
+++ b/transformation_workbook.xlsx
@@ -476,7 +476,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13.5" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
@@ -2788,7 +2788,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13.5" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
@@ -3558,7 +3558,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13.5" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
@@ -4360,7 +4360,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13.5" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
@@ -5929,7 +5929,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13.5" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
@@ -6492,7 +6492,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13.5" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
@@ -7062,7 +7062,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13.5" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="7.33203125" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -7626,7 +7626,7 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13.5" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
@@ -8382,7 +8382,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13.5" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="5" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -10820,7 +10820,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V33"/>
+  <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10946,6 +10946,94 @@
           <t>Detroit</t>
         </is>
       </c>
+      <c r="B2">
+        <f>INDEX('Points Per Game'!B:B, MATCH(A2, 'Points Per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="C2">
+        <f>INDEX('Rushing Attempts per Game'!B:B, MATCH(A2, 'Rushing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="D2">
+        <f>INDEX('Rushing Yards per Game'!B:B, MATCH(A2, 'Rushing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="E2">
+        <f>INDEX('Rushing Touchdowns %'!B:B, MATCH(A2, 'Rushing Touchdowns %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="F2">
+        <f>INDEX('Yards per Rush Attempt'!B:B, MATCH(A2, 'Yards per Rush Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="G2">
+        <f>INDEX('Rushing Play % (2023)'!B:B, MATCH(A2, 'Rushing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="H2">
+        <f>INDEX('Rushing Play % (2013)'!B:B, MATCH(A2, 'Rushing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="I2">
+        <f>INDEX('Rushing Play % (2003)'!B:B, MATCH(A2, 'Rushing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="J2">
+        <f>INDEX('Passing Attempts per Game'!B:B, MATCH(A2, 'Passing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="K2">
+        <f>INDEX('Passing Yards per Game'!B:B, MATCH(A2, 'Passing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="L2">
+        <f>INDEX('Passing Touchdown %'!B:B, MATCH(A2, 'Passing Touchdown %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="M2">
+        <f>INDEX('Yards per Pass Attempt'!B:B, MATCH(A2, 'Yards per Pass Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="N2">
+        <f>INDEX('Passing Play % (2023)'!B:B, MATCH(A2, 'Passing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="O2">
+        <f>INDEX('Passing Play % (2013)'!B:B, MATCH(A2, 'Passing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="P2">
+        <f>INDEX('Passing Play % (2003)'!B:B, MATCH(A2, 'Passing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="Q2">
+        <f>INDEX('Win % (2023)'!B:B, MATCH(A2, 'Win % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="R2">
+        <f>INDEX('Win % (2013)'!B:B, MATCH(A2, 'Win % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="S2">
+        <f>INDEX('Win % (2003)'!B:B, MATCH(A2, 'Win % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="T2">
+        <f>INDEX('Completion % (2023)'!B:B, MATCH(A2, 'Completion % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="U2">
+        <f>INDEX('Completion % (2013)'!B:B, MATCH(A2, 'Completion % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="V2">
+        <f>INDEX('Completion % (2003)'!B:B, MATCH(A2, 'Completion % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="W2">
+        <f>INDEX('merged_data_python'!B:B, MATCH(A2, 'merged_data_python'!A:A, 0))</f>
+        <v/>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -10953,6 +11041,94 @@
           <t>Washington</t>
         </is>
       </c>
+      <c r="B3">
+        <f>INDEX('Points Per Game'!B:B, MATCH(A3, 'Points Per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="C3">
+        <f>INDEX('Rushing Attempts per Game'!B:B, MATCH(A3, 'Rushing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="D3">
+        <f>INDEX('Rushing Yards per Game'!B:B, MATCH(A3, 'Rushing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="E3">
+        <f>INDEX('Rushing Touchdowns %'!B:B, MATCH(A3, 'Rushing Touchdowns %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="F3">
+        <f>INDEX('Yards per Rush Attempt'!B:B, MATCH(A3, 'Yards per Rush Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="G3">
+        <f>INDEX('Rushing Play % (2023)'!B:B, MATCH(A3, 'Rushing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="H3">
+        <f>INDEX('Rushing Play % (2013)'!B:B, MATCH(A3, 'Rushing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="I3">
+        <f>INDEX('Rushing Play % (2003)'!B:B, MATCH(A3, 'Rushing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="J3">
+        <f>INDEX('Passing Attempts per Game'!B:B, MATCH(A3, 'Passing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="K3">
+        <f>INDEX('Passing Yards per Game'!B:B, MATCH(A3, 'Passing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="L3">
+        <f>INDEX('Passing Touchdown %'!B:B, MATCH(A3, 'Passing Touchdown %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="M3">
+        <f>INDEX('Yards per Pass Attempt'!B:B, MATCH(A3, 'Yards per Pass Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="N3">
+        <f>INDEX('Passing Play % (2023)'!B:B, MATCH(A3, 'Passing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="O3">
+        <f>INDEX('Passing Play % (2013)'!B:B, MATCH(A3, 'Passing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="P3">
+        <f>INDEX('Passing Play % (2003)'!B:B, MATCH(A3, 'Passing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="Q3">
+        <f>INDEX('Win % (2023)'!B:B, MATCH(A3, 'Win % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="R3">
+        <f>INDEX('Win % (2013)'!B:B, MATCH(A3, 'Win % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="S3">
+        <f>INDEX('Win % (2003)'!B:B, MATCH(A3, 'Win % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="T3">
+        <f>INDEX('Completion % (2023)'!B:B, MATCH(A3, 'Completion % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="U3">
+        <f>INDEX('Completion % (2013)'!B:B, MATCH(A3, 'Completion % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="V3">
+        <f>INDEX('Completion % (2003)'!B:B, MATCH(A3, 'Completion % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="W3">
+        <f>INDEX('merged_data_python'!B:B, MATCH(A3, 'merged_data_python'!A:A, 0))</f>
+        <v/>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -10960,6 +11136,94 @@
           <t>Tampa Bay</t>
         </is>
       </c>
+      <c r="B4">
+        <f>INDEX('Points Per Game'!B:B, MATCH(A4, 'Points Per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="C4">
+        <f>INDEX('Rushing Attempts per Game'!B:B, MATCH(A4, 'Rushing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="D4">
+        <f>INDEX('Rushing Yards per Game'!B:B, MATCH(A4, 'Rushing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="E4">
+        <f>INDEX('Rushing Touchdowns %'!B:B, MATCH(A4, 'Rushing Touchdowns %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="F4">
+        <f>INDEX('Yards per Rush Attempt'!B:B, MATCH(A4, 'Yards per Rush Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="G4">
+        <f>INDEX('Rushing Play % (2023)'!B:B, MATCH(A4, 'Rushing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="H4">
+        <f>INDEX('Rushing Play % (2013)'!B:B, MATCH(A4, 'Rushing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="I4">
+        <f>INDEX('Rushing Play % (2003)'!B:B, MATCH(A4, 'Rushing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="J4">
+        <f>INDEX('Passing Attempts per Game'!B:B, MATCH(A4, 'Passing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="K4">
+        <f>INDEX('Passing Yards per Game'!B:B, MATCH(A4, 'Passing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="L4">
+        <f>INDEX('Passing Touchdown %'!B:B, MATCH(A4, 'Passing Touchdown %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="M4">
+        <f>INDEX('Yards per Pass Attempt'!B:B, MATCH(A4, 'Yards per Pass Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="N4">
+        <f>INDEX('Passing Play % (2023)'!B:B, MATCH(A4, 'Passing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="O4">
+        <f>INDEX('Passing Play % (2013)'!B:B, MATCH(A4, 'Passing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="P4">
+        <f>INDEX('Passing Play % (2003)'!B:B, MATCH(A4, 'Passing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="Q4">
+        <f>INDEX('Win % (2023)'!B:B, MATCH(A4, 'Win % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="R4">
+        <f>INDEX('Win % (2013)'!B:B, MATCH(A4, 'Win % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="S4">
+        <f>INDEX('Win % (2003)'!B:B, MATCH(A4, 'Win % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="T4">
+        <f>INDEX('Completion % (2023)'!B:B, MATCH(A4, 'Completion % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="U4">
+        <f>INDEX('Completion % (2013)'!B:B, MATCH(A4, 'Completion % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="V4">
+        <f>INDEX('Completion % (2003)'!B:B, MATCH(A4, 'Completion % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="W4">
+        <f>INDEX('merged_data_python'!B:B, MATCH(A4, 'merged_data_python'!A:A, 0))</f>
+        <v/>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -10967,6 +11231,94 @@
           <t>Baltimore</t>
         </is>
       </c>
+      <c r="B5">
+        <f>INDEX('Points Per Game'!B:B, MATCH(A5, 'Points Per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="C5">
+        <f>INDEX('Rushing Attempts per Game'!B:B, MATCH(A5, 'Rushing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="D5">
+        <f>INDEX('Rushing Yards per Game'!B:B, MATCH(A5, 'Rushing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="E5">
+        <f>INDEX('Rushing Touchdowns %'!B:B, MATCH(A5, 'Rushing Touchdowns %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="F5">
+        <f>INDEX('Yards per Rush Attempt'!B:B, MATCH(A5, 'Yards per Rush Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="G5">
+        <f>INDEX('Rushing Play % (2023)'!B:B, MATCH(A5, 'Rushing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="H5">
+        <f>INDEX('Rushing Play % (2013)'!B:B, MATCH(A5, 'Rushing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="I5">
+        <f>INDEX('Rushing Play % (2003)'!B:B, MATCH(A5, 'Rushing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="J5">
+        <f>INDEX('Passing Attempts per Game'!B:B, MATCH(A5, 'Passing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="K5">
+        <f>INDEX('Passing Yards per Game'!B:B, MATCH(A5, 'Passing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="L5">
+        <f>INDEX('Passing Touchdown %'!B:B, MATCH(A5, 'Passing Touchdown %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="M5">
+        <f>INDEX('Yards per Pass Attempt'!B:B, MATCH(A5, 'Yards per Pass Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="N5">
+        <f>INDEX('Passing Play % (2023)'!B:B, MATCH(A5, 'Passing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="O5">
+        <f>INDEX('Passing Play % (2013)'!B:B, MATCH(A5, 'Passing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="P5">
+        <f>INDEX('Passing Play % (2003)'!B:B, MATCH(A5, 'Passing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="Q5">
+        <f>INDEX('Win % (2023)'!B:B, MATCH(A5, 'Win % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="R5">
+        <f>INDEX('Win % (2013)'!B:B, MATCH(A5, 'Win % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="S5">
+        <f>INDEX('Win % (2003)'!B:B, MATCH(A5, 'Win % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="T5">
+        <f>INDEX('Completion % (2023)'!B:B, MATCH(A5, 'Completion % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="U5">
+        <f>INDEX('Completion % (2013)'!B:B, MATCH(A5, 'Completion % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="V5">
+        <f>INDEX('Completion % (2003)'!B:B, MATCH(A5, 'Completion % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="W5">
+        <f>INDEX('merged_data_python'!B:B, MATCH(A5, 'merged_data_python'!A:A, 0))</f>
+        <v/>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -10974,6 +11326,94 @@
           <t>Minnesota</t>
         </is>
       </c>
+      <c r="B6">
+        <f>INDEX('Points Per Game'!B:B, MATCH(A6, 'Points Per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="C6">
+        <f>INDEX('Rushing Attempts per Game'!B:B, MATCH(A6, 'Rushing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="D6">
+        <f>INDEX('Rushing Yards per Game'!B:B, MATCH(A6, 'Rushing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="E6">
+        <f>INDEX('Rushing Touchdowns %'!B:B, MATCH(A6, 'Rushing Touchdowns %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="F6">
+        <f>INDEX('Yards per Rush Attempt'!B:B, MATCH(A6, 'Yards per Rush Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="G6">
+        <f>INDEX('Rushing Play % (2023)'!B:B, MATCH(A6, 'Rushing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="H6">
+        <f>INDEX('Rushing Play % (2013)'!B:B, MATCH(A6, 'Rushing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="I6">
+        <f>INDEX('Rushing Play % (2003)'!B:B, MATCH(A6, 'Rushing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="J6">
+        <f>INDEX('Passing Attempts per Game'!B:B, MATCH(A6, 'Passing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="K6">
+        <f>INDEX('Passing Yards per Game'!B:B, MATCH(A6, 'Passing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="L6">
+        <f>INDEX('Passing Touchdown %'!B:B, MATCH(A6, 'Passing Touchdown %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="M6">
+        <f>INDEX('Yards per Pass Attempt'!B:B, MATCH(A6, 'Yards per Pass Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="N6">
+        <f>INDEX('Passing Play % (2023)'!B:B, MATCH(A6, 'Passing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="O6">
+        <f>INDEX('Passing Play % (2013)'!B:B, MATCH(A6, 'Passing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="P6">
+        <f>INDEX('Passing Play % (2003)'!B:B, MATCH(A6, 'Passing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="Q6">
+        <f>INDEX('Win % (2023)'!B:B, MATCH(A6, 'Win % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="R6">
+        <f>INDEX('Win % (2013)'!B:B, MATCH(A6, 'Win % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="S6">
+        <f>INDEX('Win % (2003)'!B:B, MATCH(A6, 'Win % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="T6">
+        <f>INDEX('Completion % (2023)'!B:B, MATCH(A6, 'Completion % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="U6">
+        <f>INDEX('Completion % (2013)'!B:B, MATCH(A6, 'Completion % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="V6">
+        <f>INDEX('Completion % (2003)'!B:B, MATCH(A6, 'Completion % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="W6">
+        <f>INDEX('merged_data_python'!B:B, MATCH(A6, 'merged_data_python'!A:A, 0))</f>
+        <v/>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -10981,6 +11421,94 @@
           <t>Buffalo</t>
         </is>
       </c>
+      <c r="B7">
+        <f>INDEX('Points Per Game'!B:B, MATCH(A7, 'Points Per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="C7">
+        <f>INDEX('Rushing Attempts per Game'!B:B, MATCH(A7, 'Rushing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="D7">
+        <f>INDEX('Rushing Yards per Game'!B:B, MATCH(A7, 'Rushing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="E7">
+        <f>INDEX('Rushing Touchdowns %'!B:B, MATCH(A7, 'Rushing Touchdowns %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="F7">
+        <f>INDEX('Yards per Rush Attempt'!B:B, MATCH(A7, 'Yards per Rush Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="G7">
+        <f>INDEX('Rushing Play % (2023)'!B:B, MATCH(A7, 'Rushing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="H7">
+        <f>INDEX('Rushing Play % (2013)'!B:B, MATCH(A7, 'Rushing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="I7">
+        <f>INDEX('Rushing Play % (2003)'!B:B, MATCH(A7, 'Rushing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="J7">
+        <f>INDEX('Passing Attempts per Game'!B:B, MATCH(A7, 'Passing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="K7">
+        <f>INDEX('Passing Yards per Game'!B:B, MATCH(A7, 'Passing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="L7">
+        <f>INDEX('Passing Touchdown %'!B:B, MATCH(A7, 'Passing Touchdown %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="M7">
+        <f>INDEX('Yards per Pass Attempt'!B:B, MATCH(A7, 'Yards per Pass Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="N7">
+        <f>INDEX('Passing Play % (2023)'!B:B, MATCH(A7, 'Passing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="O7">
+        <f>INDEX('Passing Play % (2013)'!B:B, MATCH(A7, 'Passing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="P7">
+        <f>INDEX('Passing Play % (2003)'!B:B, MATCH(A7, 'Passing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="Q7">
+        <f>INDEX('Win % (2023)'!B:B, MATCH(A7, 'Win % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="R7">
+        <f>INDEX('Win % (2013)'!B:B, MATCH(A7, 'Win % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="S7">
+        <f>INDEX('Win % (2003)'!B:B, MATCH(A7, 'Win % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="T7">
+        <f>INDEX('Completion % (2023)'!B:B, MATCH(A7, 'Completion % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="U7">
+        <f>INDEX('Completion % (2013)'!B:B, MATCH(A7, 'Completion % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="V7">
+        <f>INDEX('Completion % (2003)'!B:B, MATCH(A7, 'Completion % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="W7">
+        <f>INDEX('merged_data_python'!B:B, MATCH(A7, 'merged_data_python'!A:A, 0))</f>
+        <v/>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -10988,6 +11516,94 @@
           <t>San Francisco</t>
         </is>
       </c>
+      <c r="B8">
+        <f>INDEX('Points Per Game'!B:B, MATCH(A8, 'Points Per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="C8">
+        <f>INDEX('Rushing Attempts per Game'!B:B, MATCH(A8, 'Rushing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="D8">
+        <f>INDEX('Rushing Yards per Game'!B:B, MATCH(A8, 'Rushing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="E8">
+        <f>INDEX('Rushing Touchdowns %'!B:B, MATCH(A8, 'Rushing Touchdowns %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="F8">
+        <f>INDEX('Yards per Rush Attempt'!B:B, MATCH(A8, 'Yards per Rush Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="G8">
+        <f>INDEX('Rushing Play % (2023)'!B:B, MATCH(A8, 'Rushing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="H8">
+        <f>INDEX('Rushing Play % (2013)'!B:B, MATCH(A8, 'Rushing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="I8">
+        <f>INDEX('Rushing Play % (2003)'!B:B, MATCH(A8, 'Rushing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="J8">
+        <f>INDEX('Passing Attempts per Game'!B:B, MATCH(A8, 'Passing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="K8">
+        <f>INDEX('Passing Yards per Game'!B:B, MATCH(A8, 'Passing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="L8">
+        <f>INDEX('Passing Touchdown %'!B:B, MATCH(A8, 'Passing Touchdown %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="M8">
+        <f>INDEX('Yards per Pass Attempt'!B:B, MATCH(A8, 'Yards per Pass Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="N8">
+        <f>INDEX('Passing Play % (2023)'!B:B, MATCH(A8, 'Passing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="O8">
+        <f>INDEX('Passing Play % (2013)'!B:B, MATCH(A8, 'Passing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="P8">
+        <f>INDEX('Passing Play % (2003)'!B:B, MATCH(A8, 'Passing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="Q8">
+        <f>INDEX('Win % (2023)'!B:B, MATCH(A8, 'Win % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="R8">
+        <f>INDEX('Win % (2013)'!B:B, MATCH(A8, 'Win % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="S8">
+        <f>INDEX('Win % (2003)'!B:B, MATCH(A8, 'Win % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="T8">
+        <f>INDEX('Completion % (2023)'!B:B, MATCH(A8, 'Completion % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="U8">
+        <f>INDEX('Completion % (2013)'!B:B, MATCH(A8, 'Completion % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="V8">
+        <f>INDEX('Completion % (2003)'!B:B, MATCH(A8, 'Completion % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="W8">
+        <f>INDEX('merged_data_python'!B:B, MATCH(A8, 'merged_data_python'!A:A, 0))</f>
+        <v/>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -10995,6 +11611,94 @@
           <t>Green Bay</t>
         </is>
       </c>
+      <c r="B9">
+        <f>INDEX('Points Per Game'!B:B, MATCH(A9, 'Points Per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="C9">
+        <f>INDEX('Rushing Attempts per Game'!B:B, MATCH(A9, 'Rushing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="D9">
+        <f>INDEX('Rushing Yards per Game'!B:B, MATCH(A9, 'Rushing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="E9">
+        <f>INDEX('Rushing Touchdowns %'!B:B, MATCH(A9, 'Rushing Touchdowns %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="F9">
+        <f>INDEX('Yards per Rush Attempt'!B:B, MATCH(A9, 'Yards per Rush Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="G9">
+        <f>INDEX('Rushing Play % (2023)'!B:B, MATCH(A9, 'Rushing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="H9">
+        <f>INDEX('Rushing Play % (2013)'!B:B, MATCH(A9, 'Rushing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="I9">
+        <f>INDEX('Rushing Play % (2003)'!B:B, MATCH(A9, 'Rushing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="J9">
+        <f>INDEX('Passing Attempts per Game'!B:B, MATCH(A9, 'Passing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="K9">
+        <f>INDEX('Passing Yards per Game'!B:B, MATCH(A9, 'Passing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="L9">
+        <f>INDEX('Passing Touchdown %'!B:B, MATCH(A9, 'Passing Touchdown %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="M9">
+        <f>INDEX('Yards per Pass Attempt'!B:B, MATCH(A9, 'Yards per Pass Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="N9">
+        <f>INDEX('Passing Play % (2023)'!B:B, MATCH(A9, 'Passing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="O9">
+        <f>INDEX('Passing Play % (2013)'!B:B, MATCH(A9, 'Passing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="P9">
+        <f>INDEX('Passing Play % (2003)'!B:B, MATCH(A9, 'Passing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="Q9">
+        <f>INDEX('Win % (2023)'!B:B, MATCH(A9, 'Win % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="R9">
+        <f>INDEX('Win % (2013)'!B:B, MATCH(A9, 'Win % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="S9">
+        <f>INDEX('Win % (2003)'!B:B, MATCH(A9, 'Win % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="T9">
+        <f>INDEX('Completion % (2023)'!B:B, MATCH(A9, 'Completion % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="U9">
+        <f>INDEX('Completion % (2013)'!B:B, MATCH(A9, 'Completion % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="V9">
+        <f>INDEX('Completion % (2003)'!B:B, MATCH(A9, 'Completion % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="W9">
+        <f>INDEX('merged_data_python'!B:B, MATCH(A9, 'merged_data_python'!A:A, 0))</f>
+        <v/>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -11002,6 +11706,94 @@
           <t>Cincinnati</t>
         </is>
       </c>
+      <c r="B10">
+        <f>INDEX('Points Per Game'!B:B, MATCH(A10, 'Points Per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="C10">
+        <f>INDEX('Rushing Attempts per Game'!B:B, MATCH(A10, 'Rushing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="D10">
+        <f>INDEX('Rushing Yards per Game'!B:B, MATCH(A10, 'Rushing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="E10">
+        <f>INDEX('Rushing Touchdowns %'!B:B, MATCH(A10, 'Rushing Touchdowns %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="F10">
+        <f>INDEX('Yards per Rush Attempt'!B:B, MATCH(A10, 'Yards per Rush Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="G10">
+        <f>INDEX('Rushing Play % (2023)'!B:B, MATCH(A10, 'Rushing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="H10">
+        <f>INDEX('Rushing Play % (2013)'!B:B, MATCH(A10, 'Rushing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="I10">
+        <f>INDEX('Rushing Play % (2003)'!B:B, MATCH(A10, 'Rushing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="J10">
+        <f>INDEX('Passing Attempts per Game'!B:B, MATCH(A10, 'Passing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="K10">
+        <f>INDEX('Passing Yards per Game'!B:B, MATCH(A10, 'Passing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="L10">
+        <f>INDEX('Passing Touchdown %'!B:B, MATCH(A10, 'Passing Touchdown %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="M10">
+        <f>INDEX('Yards per Pass Attempt'!B:B, MATCH(A10, 'Yards per Pass Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="N10">
+        <f>INDEX('Passing Play % (2023)'!B:B, MATCH(A10, 'Passing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="O10">
+        <f>INDEX('Passing Play % (2013)'!B:B, MATCH(A10, 'Passing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="P10">
+        <f>INDEX('Passing Play % (2003)'!B:B, MATCH(A10, 'Passing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="Q10">
+        <f>INDEX('Win % (2023)'!B:B, MATCH(A10, 'Win % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="R10">
+        <f>INDEX('Win % (2013)'!B:B, MATCH(A10, 'Win % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="S10">
+        <f>INDEX('Win % (2003)'!B:B, MATCH(A10, 'Win % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="T10">
+        <f>INDEX('Completion % (2023)'!B:B, MATCH(A10, 'Completion % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="U10">
+        <f>INDEX('Completion % (2013)'!B:B, MATCH(A10, 'Completion % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="V10">
+        <f>INDEX('Completion % (2003)'!B:B, MATCH(A10, 'Completion % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="W10">
+        <f>INDEX('merged_data_python'!B:B, MATCH(A10, 'merged_data_python'!A:A, 0))</f>
+        <v/>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -11009,6 +11801,94 @@
           <t>New Orleans</t>
         </is>
       </c>
+      <c r="B11">
+        <f>INDEX('Points Per Game'!B:B, MATCH(A11, 'Points Per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="C11">
+        <f>INDEX('Rushing Attempts per Game'!B:B, MATCH(A11, 'Rushing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="D11">
+        <f>INDEX('Rushing Yards per Game'!B:B, MATCH(A11, 'Rushing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="E11">
+        <f>INDEX('Rushing Touchdowns %'!B:B, MATCH(A11, 'Rushing Touchdowns %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="F11">
+        <f>INDEX('Yards per Rush Attempt'!B:B, MATCH(A11, 'Yards per Rush Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="G11">
+        <f>INDEX('Rushing Play % (2023)'!B:B, MATCH(A11, 'Rushing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="H11">
+        <f>INDEX('Rushing Play % (2013)'!B:B, MATCH(A11, 'Rushing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="I11">
+        <f>INDEX('Rushing Play % (2003)'!B:B, MATCH(A11, 'Rushing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="J11">
+        <f>INDEX('Passing Attempts per Game'!B:B, MATCH(A11, 'Passing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="K11">
+        <f>INDEX('Passing Yards per Game'!B:B, MATCH(A11, 'Passing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="L11">
+        <f>INDEX('Passing Touchdown %'!B:B, MATCH(A11, 'Passing Touchdown %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="M11">
+        <f>INDEX('Yards per Pass Attempt'!B:B, MATCH(A11, 'Yards per Pass Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="N11">
+        <f>INDEX('Passing Play % (2023)'!B:B, MATCH(A11, 'Passing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="O11">
+        <f>INDEX('Passing Play % (2013)'!B:B, MATCH(A11, 'Passing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="P11">
+        <f>INDEX('Passing Play % (2003)'!B:B, MATCH(A11, 'Passing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="Q11">
+        <f>INDEX('Win % (2023)'!B:B, MATCH(A11, 'Win % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="R11">
+        <f>INDEX('Win % (2013)'!B:B, MATCH(A11, 'Win % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="S11">
+        <f>INDEX('Win % (2003)'!B:B, MATCH(A11, 'Win % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="T11">
+        <f>INDEX('Completion % (2023)'!B:B, MATCH(A11, 'Completion % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="U11">
+        <f>INDEX('Completion % (2013)'!B:B, MATCH(A11, 'Completion % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="V11">
+        <f>INDEX('Completion % (2003)'!B:B, MATCH(A11, 'Completion % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="W11">
+        <f>INDEX('merged_data_python'!B:B, MATCH(A11, 'merged_data_python'!A:A, 0))</f>
+        <v/>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -11016,6 +11896,94 @@
           <t>Atlanta</t>
         </is>
       </c>
+      <c r="B12">
+        <f>INDEX('Points Per Game'!B:B, MATCH(A12, 'Points Per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="C12">
+        <f>INDEX('Rushing Attempts per Game'!B:B, MATCH(A12, 'Rushing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="D12">
+        <f>INDEX('Rushing Yards per Game'!B:B, MATCH(A12, 'Rushing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="E12">
+        <f>INDEX('Rushing Touchdowns %'!B:B, MATCH(A12, 'Rushing Touchdowns %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="F12">
+        <f>INDEX('Yards per Rush Attempt'!B:B, MATCH(A12, 'Yards per Rush Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="G12">
+        <f>INDEX('Rushing Play % (2023)'!B:B, MATCH(A12, 'Rushing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="H12">
+        <f>INDEX('Rushing Play % (2013)'!B:B, MATCH(A12, 'Rushing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="I12">
+        <f>INDEX('Rushing Play % (2003)'!B:B, MATCH(A12, 'Rushing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="J12">
+        <f>INDEX('Passing Attempts per Game'!B:B, MATCH(A12, 'Passing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="K12">
+        <f>INDEX('Passing Yards per Game'!B:B, MATCH(A12, 'Passing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="L12">
+        <f>INDEX('Passing Touchdown %'!B:B, MATCH(A12, 'Passing Touchdown %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="M12">
+        <f>INDEX('Yards per Pass Attempt'!B:B, MATCH(A12, 'Yards per Pass Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="N12">
+        <f>INDEX('Passing Play % (2023)'!B:B, MATCH(A12, 'Passing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="O12">
+        <f>INDEX('Passing Play % (2013)'!B:B, MATCH(A12, 'Passing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="P12">
+        <f>INDEX('Passing Play % (2003)'!B:B, MATCH(A12, 'Passing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="Q12">
+        <f>INDEX('Win % (2023)'!B:B, MATCH(A12, 'Win % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="R12">
+        <f>INDEX('Win % (2013)'!B:B, MATCH(A12, 'Win % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="S12">
+        <f>INDEX('Win % (2003)'!B:B, MATCH(A12, 'Win % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="T12">
+        <f>INDEX('Completion % (2023)'!B:B, MATCH(A12, 'Completion % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="U12">
+        <f>INDEX('Completion % (2013)'!B:B, MATCH(A12, 'Completion % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="V12">
+        <f>INDEX('Completion % (2003)'!B:B, MATCH(A12, 'Completion % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="W12">
+        <f>INDEX('merged_data_python'!B:B, MATCH(A12, 'merged_data_python'!A:A, 0))</f>
+        <v/>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -11023,6 +11991,94 @@
           <t>Chicago</t>
         </is>
       </c>
+      <c r="B13">
+        <f>INDEX('Points Per Game'!B:B, MATCH(A13, 'Points Per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="C13">
+        <f>INDEX('Rushing Attempts per Game'!B:B, MATCH(A13, 'Rushing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="D13">
+        <f>INDEX('Rushing Yards per Game'!B:B, MATCH(A13, 'Rushing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="E13">
+        <f>INDEX('Rushing Touchdowns %'!B:B, MATCH(A13, 'Rushing Touchdowns %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="F13">
+        <f>INDEX('Yards per Rush Attempt'!B:B, MATCH(A13, 'Yards per Rush Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="G13">
+        <f>INDEX('Rushing Play % (2023)'!B:B, MATCH(A13, 'Rushing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="H13">
+        <f>INDEX('Rushing Play % (2013)'!B:B, MATCH(A13, 'Rushing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="I13">
+        <f>INDEX('Rushing Play % (2003)'!B:B, MATCH(A13, 'Rushing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="J13">
+        <f>INDEX('Passing Attempts per Game'!B:B, MATCH(A13, 'Passing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="K13">
+        <f>INDEX('Passing Yards per Game'!B:B, MATCH(A13, 'Passing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="L13">
+        <f>INDEX('Passing Touchdown %'!B:B, MATCH(A13, 'Passing Touchdown %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="M13">
+        <f>INDEX('Yards per Pass Attempt'!B:B, MATCH(A13, 'Yards per Pass Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="N13">
+        <f>INDEX('Passing Play % (2023)'!B:B, MATCH(A13, 'Passing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="O13">
+        <f>INDEX('Passing Play % (2013)'!B:B, MATCH(A13, 'Passing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="P13">
+        <f>INDEX('Passing Play % (2003)'!B:B, MATCH(A13, 'Passing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="Q13">
+        <f>INDEX('Win % (2023)'!B:B, MATCH(A13, 'Win % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="R13">
+        <f>INDEX('Win % (2013)'!B:B, MATCH(A13, 'Win % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="S13">
+        <f>INDEX('Win % (2003)'!B:B, MATCH(A13, 'Win % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="T13">
+        <f>INDEX('Completion % (2023)'!B:B, MATCH(A13, 'Completion % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="U13">
+        <f>INDEX('Completion % (2013)'!B:B, MATCH(A13, 'Completion % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="V13">
+        <f>INDEX('Completion % (2003)'!B:B, MATCH(A13, 'Completion % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="W13">
+        <f>INDEX('merged_data_python'!B:B, MATCH(A13, 'merged_data_python'!A:A, 0))</f>
+        <v/>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -11030,6 +12086,94 @@
           <t>Seattle</t>
         </is>
       </c>
+      <c r="B14">
+        <f>INDEX('Points Per Game'!B:B, MATCH(A14, 'Points Per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="C14">
+        <f>INDEX('Rushing Attempts per Game'!B:B, MATCH(A14, 'Rushing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="D14">
+        <f>INDEX('Rushing Yards per Game'!B:B, MATCH(A14, 'Rushing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="E14">
+        <f>INDEX('Rushing Touchdowns %'!B:B, MATCH(A14, 'Rushing Touchdowns %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="F14">
+        <f>INDEX('Yards per Rush Attempt'!B:B, MATCH(A14, 'Yards per Rush Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="G14">
+        <f>INDEX('Rushing Play % (2023)'!B:B, MATCH(A14, 'Rushing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="H14">
+        <f>INDEX('Rushing Play % (2013)'!B:B, MATCH(A14, 'Rushing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="I14">
+        <f>INDEX('Rushing Play % (2003)'!B:B, MATCH(A14, 'Rushing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="J14">
+        <f>INDEX('Passing Attempts per Game'!B:B, MATCH(A14, 'Passing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="K14">
+        <f>INDEX('Passing Yards per Game'!B:B, MATCH(A14, 'Passing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="L14">
+        <f>INDEX('Passing Touchdown %'!B:B, MATCH(A14, 'Passing Touchdown %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="M14">
+        <f>INDEX('Yards per Pass Attempt'!B:B, MATCH(A14, 'Yards per Pass Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="N14">
+        <f>INDEX('Passing Play % (2023)'!B:B, MATCH(A14, 'Passing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="O14">
+        <f>INDEX('Passing Play % (2013)'!B:B, MATCH(A14, 'Passing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="P14">
+        <f>INDEX('Passing Play % (2003)'!B:B, MATCH(A14, 'Passing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="Q14">
+        <f>INDEX('Win % (2023)'!B:B, MATCH(A14, 'Win % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="R14">
+        <f>INDEX('Win % (2013)'!B:B, MATCH(A14, 'Win % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="S14">
+        <f>INDEX('Win % (2003)'!B:B, MATCH(A14, 'Win % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="T14">
+        <f>INDEX('Completion % (2023)'!B:B, MATCH(A14, 'Completion % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="U14">
+        <f>INDEX('Completion % (2013)'!B:B, MATCH(A14, 'Completion % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="V14">
+        <f>INDEX('Completion % (2003)'!B:B, MATCH(A14, 'Completion % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="W14">
+        <f>INDEX('merged_data_python'!B:B, MATCH(A14, 'merged_data_python'!A:A, 0))</f>
+        <v/>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -11037,6 +12181,94 @@
           <t>Houston</t>
         </is>
       </c>
+      <c r="B15">
+        <f>INDEX('Points Per Game'!B:B, MATCH(A15, 'Points Per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="C15">
+        <f>INDEX('Rushing Attempts per Game'!B:B, MATCH(A15, 'Rushing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="D15">
+        <f>INDEX('Rushing Yards per Game'!B:B, MATCH(A15, 'Rushing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="E15">
+        <f>INDEX('Rushing Touchdowns %'!B:B, MATCH(A15, 'Rushing Touchdowns %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="F15">
+        <f>INDEX('Yards per Rush Attempt'!B:B, MATCH(A15, 'Yards per Rush Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="G15">
+        <f>INDEX('Rushing Play % (2023)'!B:B, MATCH(A15, 'Rushing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="H15">
+        <f>INDEX('Rushing Play % (2013)'!B:B, MATCH(A15, 'Rushing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="I15">
+        <f>INDEX('Rushing Play % (2003)'!B:B, MATCH(A15, 'Rushing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="J15">
+        <f>INDEX('Passing Attempts per Game'!B:B, MATCH(A15, 'Passing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="K15">
+        <f>INDEX('Passing Yards per Game'!B:B, MATCH(A15, 'Passing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="L15">
+        <f>INDEX('Passing Touchdown %'!B:B, MATCH(A15, 'Passing Touchdown %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="M15">
+        <f>INDEX('Yards per Pass Attempt'!B:B, MATCH(A15, 'Yards per Pass Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="N15">
+        <f>INDEX('Passing Play % (2023)'!B:B, MATCH(A15, 'Passing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="O15">
+        <f>INDEX('Passing Play % (2013)'!B:B, MATCH(A15, 'Passing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="P15">
+        <f>INDEX('Passing Play % (2003)'!B:B, MATCH(A15, 'Passing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="Q15">
+        <f>INDEX('Win % (2023)'!B:B, MATCH(A15, 'Win % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="R15">
+        <f>INDEX('Win % (2013)'!B:B, MATCH(A15, 'Win % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="S15">
+        <f>INDEX('Win % (2003)'!B:B, MATCH(A15, 'Win % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="T15">
+        <f>INDEX('Completion % (2023)'!B:B, MATCH(A15, 'Completion % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="U15">
+        <f>INDEX('Completion % (2013)'!B:B, MATCH(A15, 'Completion % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="V15">
+        <f>INDEX('Completion % (2003)'!B:B, MATCH(A15, 'Completion % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="W15">
+        <f>INDEX('merged_data_python'!B:B, MATCH(A15, 'merged_data_python'!A:A, 0))</f>
+        <v/>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -11044,6 +12276,94 @@
           <t>Kansas City</t>
         </is>
       </c>
+      <c r="B16">
+        <f>INDEX('Points Per Game'!B:B, MATCH(A16, 'Points Per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="C16">
+        <f>INDEX('Rushing Attempts per Game'!B:B, MATCH(A16, 'Rushing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="D16">
+        <f>INDEX('Rushing Yards per Game'!B:B, MATCH(A16, 'Rushing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="E16">
+        <f>INDEX('Rushing Touchdowns %'!B:B, MATCH(A16, 'Rushing Touchdowns %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="F16">
+        <f>INDEX('Yards per Rush Attempt'!B:B, MATCH(A16, 'Yards per Rush Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="G16">
+        <f>INDEX('Rushing Play % (2023)'!B:B, MATCH(A16, 'Rushing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="H16">
+        <f>INDEX('Rushing Play % (2013)'!B:B, MATCH(A16, 'Rushing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="I16">
+        <f>INDEX('Rushing Play % (2003)'!B:B, MATCH(A16, 'Rushing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="J16">
+        <f>INDEX('Passing Attempts per Game'!B:B, MATCH(A16, 'Passing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="K16">
+        <f>INDEX('Passing Yards per Game'!B:B, MATCH(A16, 'Passing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="L16">
+        <f>INDEX('Passing Touchdown %'!B:B, MATCH(A16, 'Passing Touchdown %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="M16">
+        <f>INDEX('Yards per Pass Attempt'!B:B, MATCH(A16, 'Yards per Pass Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="N16">
+        <f>INDEX('Passing Play % (2023)'!B:B, MATCH(A16, 'Passing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="O16">
+        <f>INDEX('Passing Play % (2013)'!B:B, MATCH(A16, 'Passing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="P16">
+        <f>INDEX('Passing Play % (2003)'!B:B, MATCH(A16, 'Passing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="Q16">
+        <f>INDEX('Win % (2023)'!B:B, MATCH(A16, 'Win % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="R16">
+        <f>INDEX('Win % (2013)'!B:B, MATCH(A16, 'Win % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="S16">
+        <f>INDEX('Win % (2003)'!B:B, MATCH(A16, 'Win % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="T16">
+        <f>INDEX('Completion % (2023)'!B:B, MATCH(A16, 'Completion % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="U16">
+        <f>INDEX('Completion % (2013)'!B:B, MATCH(A16, 'Completion % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="V16">
+        <f>INDEX('Completion % (2003)'!B:B, MATCH(A16, 'Completion % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="W16">
+        <f>INDEX('merged_data_python'!B:B, MATCH(A16, 'merged_data_python'!A:A, 0))</f>
+        <v/>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -11051,6 +12371,94 @@
           <t>Indianapolis</t>
         </is>
       </c>
+      <c r="B17">
+        <f>INDEX('Points Per Game'!B:B, MATCH(A17, 'Points Per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="C17">
+        <f>INDEX('Rushing Attempts per Game'!B:B, MATCH(A17, 'Rushing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="D17">
+        <f>INDEX('Rushing Yards per Game'!B:B, MATCH(A17, 'Rushing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="E17">
+        <f>INDEX('Rushing Touchdowns %'!B:B, MATCH(A17, 'Rushing Touchdowns %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="F17">
+        <f>INDEX('Yards per Rush Attempt'!B:B, MATCH(A17, 'Yards per Rush Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="G17">
+        <f>INDEX('Rushing Play % (2023)'!B:B, MATCH(A17, 'Rushing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="H17">
+        <f>INDEX('Rushing Play % (2013)'!B:B, MATCH(A17, 'Rushing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="I17">
+        <f>INDEX('Rushing Play % (2003)'!B:B, MATCH(A17, 'Rushing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="J17">
+        <f>INDEX('Passing Attempts per Game'!B:B, MATCH(A17, 'Passing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="K17">
+        <f>INDEX('Passing Yards per Game'!B:B, MATCH(A17, 'Passing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="L17">
+        <f>INDEX('Passing Touchdown %'!B:B, MATCH(A17, 'Passing Touchdown %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="M17">
+        <f>INDEX('Yards per Pass Attempt'!B:B, MATCH(A17, 'Yards per Pass Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="N17">
+        <f>INDEX('Passing Play % (2023)'!B:B, MATCH(A17, 'Passing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="O17">
+        <f>INDEX('Passing Play % (2013)'!B:B, MATCH(A17, 'Passing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="P17">
+        <f>INDEX('Passing Play % (2003)'!B:B, MATCH(A17, 'Passing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="Q17">
+        <f>INDEX('Win % (2023)'!B:B, MATCH(A17, 'Win % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="R17">
+        <f>INDEX('Win % (2013)'!B:B, MATCH(A17, 'Win % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="S17">
+        <f>INDEX('Win % (2003)'!B:B, MATCH(A17, 'Win % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="T17">
+        <f>INDEX('Completion % (2023)'!B:B, MATCH(A17, 'Completion % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="U17">
+        <f>INDEX('Completion % (2013)'!B:B, MATCH(A17, 'Completion % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="V17">
+        <f>INDEX('Completion % (2003)'!B:B, MATCH(A17, 'Completion % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="W17">
+        <f>INDEX('merged_data_python'!B:B, MATCH(A17, 'merged_data_python'!A:A, 0))</f>
+        <v/>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -11058,6 +12466,94 @@
           <t>Arizona</t>
         </is>
       </c>
+      <c r="B18">
+        <f>INDEX('Points Per Game'!B:B, MATCH(A18, 'Points Per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="C18">
+        <f>INDEX('Rushing Attempts per Game'!B:B, MATCH(A18, 'Rushing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="D18">
+        <f>INDEX('Rushing Yards per Game'!B:B, MATCH(A18, 'Rushing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="E18">
+        <f>INDEX('Rushing Touchdowns %'!B:B, MATCH(A18, 'Rushing Touchdowns %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="F18">
+        <f>INDEX('Yards per Rush Attempt'!B:B, MATCH(A18, 'Yards per Rush Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="G18">
+        <f>INDEX('Rushing Play % (2023)'!B:B, MATCH(A18, 'Rushing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="H18">
+        <f>INDEX('Rushing Play % (2013)'!B:B, MATCH(A18, 'Rushing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="I18">
+        <f>INDEX('Rushing Play % (2003)'!B:B, MATCH(A18, 'Rushing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="J18">
+        <f>INDEX('Passing Attempts per Game'!B:B, MATCH(A18, 'Passing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="K18">
+        <f>INDEX('Passing Yards per Game'!B:B, MATCH(A18, 'Passing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="L18">
+        <f>INDEX('Passing Touchdown %'!B:B, MATCH(A18, 'Passing Touchdown %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="M18">
+        <f>INDEX('Yards per Pass Attempt'!B:B, MATCH(A18, 'Yards per Pass Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="N18">
+        <f>INDEX('Passing Play % (2023)'!B:B, MATCH(A18, 'Passing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="O18">
+        <f>INDEX('Passing Play % (2013)'!B:B, MATCH(A18, 'Passing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="P18">
+        <f>INDEX('Passing Play % (2003)'!B:B, MATCH(A18, 'Passing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="Q18">
+        <f>INDEX('Win % (2023)'!B:B, MATCH(A18, 'Win % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="R18">
+        <f>INDEX('Win % (2013)'!B:B, MATCH(A18, 'Win % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="S18">
+        <f>INDEX('Win % (2003)'!B:B, MATCH(A18, 'Win % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="T18">
+        <f>INDEX('Completion % (2023)'!B:B, MATCH(A18, 'Completion % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="U18">
+        <f>INDEX('Completion % (2013)'!B:B, MATCH(A18, 'Completion % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="V18">
+        <f>INDEX('Completion % (2003)'!B:B, MATCH(A18, 'Completion % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="W18">
+        <f>INDEX('merged_data_python'!B:B, MATCH(A18, 'merged_data_python'!A:A, 0))</f>
+        <v/>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -11065,6 +12561,94 @@
           <t>Philadelphia</t>
         </is>
       </c>
+      <c r="B19">
+        <f>INDEX('Points Per Game'!B:B, MATCH(A19, 'Points Per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="C19">
+        <f>INDEX('Rushing Attempts per Game'!B:B, MATCH(A19, 'Rushing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="D19">
+        <f>INDEX('Rushing Yards per Game'!B:B, MATCH(A19, 'Rushing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="E19">
+        <f>INDEX('Rushing Touchdowns %'!B:B, MATCH(A19, 'Rushing Touchdowns %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="F19">
+        <f>INDEX('Yards per Rush Attempt'!B:B, MATCH(A19, 'Yards per Rush Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="G19">
+        <f>INDEX('Rushing Play % (2023)'!B:B, MATCH(A19, 'Rushing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="H19">
+        <f>INDEX('Rushing Play % (2013)'!B:B, MATCH(A19, 'Rushing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="I19">
+        <f>INDEX('Rushing Play % (2003)'!B:B, MATCH(A19, 'Rushing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="J19">
+        <f>INDEX('Passing Attempts per Game'!B:B, MATCH(A19, 'Passing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="K19">
+        <f>INDEX('Passing Yards per Game'!B:B, MATCH(A19, 'Passing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="L19">
+        <f>INDEX('Passing Touchdown %'!B:B, MATCH(A19, 'Passing Touchdown %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="M19">
+        <f>INDEX('Yards per Pass Attempt'!B:B, MATCH(A19, 'Yards per Pass Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="N19">
+        <f>INDEX('Passing Play % (2023)'!B:B, MATCH(A19, 'Passing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="O19">
+        <f>INDEX('Passing Play % (2013)'!B:B, MATCH(A19, 'Passing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="P19">
+        <f>INDEX('Passing Play % (2003)'!B:B, MATCH(A19, 'Passing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="Q19">
+        <f>INDEX('Win % (2023)'!B:B, MATCH(A19, 'Win % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="R19">
+        <f>INDEX('Win % (2013)'!B:B, MATCH(A19, 'Win % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="S19">
+        <f>INDEX('Win % (2003)'!B:B, MATCH(A19, 'Win % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="T19">
+        <f>INDEX('Completion % (2023)'!B:B, MATCH(A19, 'Completion % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="U19">
+        <f>INDEX('Completion % (2013)'!B:B, MATCH(A19, 'Completion % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="V19">
+        <f>INDEX('Completion % (2003)'!B:B, MATCH(A19, 'Completion % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="W19">
+        <f>INDEX('merged_data_python'!B:B, MATCH(A19, 'merged_data_python'!A:A, 0))</f>
+        <v/>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -11072,6 +12656,94 @@
           <t>Dallas</t>
         </is>
       </c>
+      <c r="B20">
+        <f>INDEX('Points Per Game'!B:B, MATCH(A20, 'Points Per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="C20">
+        <f>INDEX('Rushing Attempts per Game'!B:B, MATCH(A20, 'Rushing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="D20">
+        <f>INDEX('Rushing Yards per Game'!B:B, MATCH(A20, 'Rushing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="E20">
+        <f>INDEX('Rushing Touchdowns %'!B:B, MATCH(A20, 'Rushing Touchdowns %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="F20">
+        <f>INDEX('Yards per Rush Attempt'!B:B, MATCH(A20, 'Yards per Rush Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="G20">
+        <f>INDEX('Rushing Play % (2023)'!B:B, MATCH(A20, 'Rushing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="H20">
+        <f>INDEX('Rushing Play % (2013)'!B:B, MATCH(A20, 'Rushing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="I20">
+        <f>INDEX('Rushing Play % (2003)'!B:B, MATCH(A20, 'Rushing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="J20">
+        <f>INDEX('Passing Attempts per Game'!B:B, MATCH(A20, 'Passing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="K20">
+        <f>INDEX('Passing Yards per Game'!B:B, MATCH(A20, 'Passing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="L20">
+        <f>INDEX('Passing Touchdown %'!B:B, MATCH(A20, 'Passing Touchdown %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="M20">
+        <f>INDEX('Yards per Pass Attempt'!B:B, MATCH(A20, 'Yards per Pass Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="N20">
+        <f>INDEX('Passing Play % (2023)'!B:B, MATCH(A20, 'Passing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="O20">
+        <f>INDEX('Passing Play % (2013)'!B:B, MATCH(A20, 'Passing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="P20">
+        <f>INDEX('Passing Play % (2003)'!B:B, MATCH(A20, 'Passing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="Q20">
+        <f>INDEX('Win % (2023)'!B:B, MATCH(A20, 'Win % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="R20">
+        <f>INDEX('Win % (2013)'!B:B, MATCH(A20, 'Win % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="S20">
+        <f>INDEX('Win % (2003)'!B:B, MATCH(A20, 'Win % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="T20">
+        <f>INDEX('Completion % (2023)'!B:B, MATCH(A20, 'Completion % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="U20">
+        <f>INDEX('Completion % (2013)'!B:B, MATCH(A20, 'Completion % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="V20">
+        <f>INDEX('Completion % (2003)'!B:B, MATCH(A20, 'Completion % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="W20">
+        <f>INDEX('merged_data_python'!B:B, MATCH(A20, 'merged_data_python'!A:A, 0))</f>
+        <v/>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -11079,6 +12751,94 @@
           <t>Denver</t>
         </is>
       </c>
+      <c r="B21">
+        <f>INDEX('Points Per Game'!B:B, MATCH(A21, 'Points Per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="C21">
+        <f>INDEX('Rushing Attempts per Game'!B:B, MATCH(A21, 'Rushing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="D21">
+        <f>INDEX('Rushing Yards per Game'!B:B, MATCH(A21, 'Rushing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="E21">
+        <f>INDEX('Rushing Touchdowns %'!B:B, MATCH(A21, 'Rushing Touchdowns %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="F21">
+        <f>INDEX('Yards per Rush Attempt'!B:B, MATCH(A21, 'Yards per Rush Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="G21">
+        <f>INDEX('Rushing Play % (2023)'!B:B, MATCH(A21, 'Rushing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="H21">
+        <f>INDEX('Rushing Play % (2013)'!B:B, MATCH(A21, 'Rushing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="I21">
+        <f>INDEX('Rushing Play % (2003)'!B:B, MATCH(A21, 'Rushing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="J21">
+        <f>INDEX('Passing Attempts per Game'!B:B, MATCH(A21, 'Passing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="K21">
+        <f>INDEX('Passing Yards per Game'!B:B, MATCH(A21, 'Passing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="L21">
+        <f>INDEX('Passing Touchdown %'!B:B, MATCH(A21, 'Passing Touchdown %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="M21">
+        <f>INDEX('Yards per Pass Attempt'!B:B, MATCH(A21, 'Yards per Pass Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="N21">
+        <f>INDEX('Passing Play % (2023)'!B:B, MATCH(A21, 'Passing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="O21">
+        <f>INDEX('Passing Play % (2013)'!B:B, MATCH(A21, 'Passing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="P21">
+        <f>INDEX('Passing Play % (2003)'!B:B, MATCH(A21, 'Passing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="Q21">
+        <f>INDEX('Win % (2023)'!B:B, MATCH(A21, 'Win % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="R21">
+        <f>INDEX('Win % (2013)'!B:B, MATCH(A21, 'Win % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="S21">
+        <f>INDEX('Win % (2003)'!B:B, MATCH(A21, 'Win % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="T21">
+        <f>INDEX('Completion % (2023)'!B:B, MATCH(A21, 'Completion % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="U21">
+        <f>INDEX('Completion % (2013)'!B:B, MATCH(A21, 'Completion % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="V21">
+        <f>INDEX('Completion % (2003)'!B:B, MATCH(A21, 'Completion % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="W21">
+        <f>INDEX('merged_data_python'!B:B, MATCH(A21, 'merged_data_python'!A:A, 0))</f>
+        <v/>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -11086,6 +12846,94 @@
           <t>Pittsburgh</t>
         </is>
       </c>
+      <c r="B22">
+        <f>INDEX('Points Per Game'!B:B, MATCH(A22, 'Points Per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="C22">
+        <f>INDEX('Rushing Attempts per Game'!B:B, MATCH(A22, 'Rushing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="D22">
+        <f>INDEX('Rushing Yards per Game'!B:B, MATCH(A22, 'Rushing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="E22">
+        <f>INDEX('Rushing Touchdowns %'!B:B, MATCH(A22, 'Rushing Touchdowns %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="F22">
+        <f>INDEX('Yards per Rush Attempt'!B:B, MATCH(A22, 'Yards per Rush Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="G22">
+        <f>INDEX('Rushing Play % (2023)'!B:B, MATCH(A22, 'Rushing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="H22">
+        <f>INDEX('Rushing Play % (2013)'!B:B, MATCH(A22, 'Rushing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="I22">
+        <f>INDEX('Rushing Play % (2003)'!B:B, MATCH(A22, 'Rushing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="J22">
+        <f>INDEX('Passing Attempts per Game'!B:B, MATCH(A22, 'Passing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="K22">
+        <f>INDEX('Passing Yards per Game'!B:B, MATCH(A22, 'Passing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="L22">
+        <f>INDEX('Passing Touchdown %'!B:B, MATCH(A22, 'Passing Touchdown %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="M22">
+        <f>INDEX('Yards per Pass Attempt'!B:B, MATCH(A22, 'Yards per Pass Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="N22">
+        <f>INDEX('Passing Play % (2023)'!B:B, MATCH(A22, 'Passing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="O22">
+        <f>INDEX('Passing Play % (2013)'!B:B, MATCH(A22, 'Passing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="P22">
+        <f>INDEX('Passing Play % (2003)'!B:B, MATCH(A22, 'Passing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="Q22">
+        <f>INDEX('Win % (2023)'!B:B, MATCH(A22, 'Win % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="R22">
+        <f>INDEX('Win % (2013)'!B:B, MATCH(A22, 'Win % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="S22">
+        <f>INDEX('Win % (2003)'!B:B, MATCH(A22, 'Win % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="T22">
+        <f>INDEX('Completion % (2023)'!B:B, MATCH(A22, 'Completion % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="U22">
+        <f>INDEX('Completion % (2013)'!B:B, MATCH(A22, 'Completion % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="V22">
+        <f>INDEX('Completion % (2003)'!B:B, MATCH(A22, 'Completion % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="W22">
+        <f>INDEX('merged_data_python'!B:B, MATCH(A22, 'merged_data_python'!A:A, 0))</f>
+        <v/>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -11093,6 +12941,94 @@
           <t>Tennessee</t>
         </is>
       </c>
+      <c r="B23">
+        <f>INDEX('Points Per Game'!B:B, MATCH(A23, 'Points Per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="C23">
+        <f>INDEX('Rushing Attempts per Game'!B:B, MATCH(A23, 'Rushing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="D23">
+        <f>INDEX('Rushing Yards per Game'!B:B, MATCH(A23, 'Rushing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="E23">
+        <f>INDEX('Rushing Touchdowns %'!B:B, MATCH(A23, 'Rushing Touchdowns %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="F23">
+        <f>INDEX('Yards per Rush Attempt'!B:B, MATCH(A23, 'Yards per Rush Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="G23">
+        <f>INDEX('Rushing Play % (2023)'!B:B, MATCH(A23, 'Rushing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="H23">
+        <f>INDEX('Rushing Play % (2013)'!B:B, MATCH(A23, 'Rushing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="I23">
+        <f>INDEX('Rushing Play % (2003)'!B:B, MATCH(A23, 'Rushing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="J23">
+        <f>INDEX('Passing Attempts per Game'!B:B, MATCH(A23, 'Passing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="K23">
+        <f>INDEX('Passing Yards per Game'!B:B, MATCH(A23, 'Passing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="L23">
+        <f>INDEX('Passing Touchdown %'!B:B, MATCH(A23, 'Passing Touchdown %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="M23">
+        <f>INDEX('Yards per Pass Attempt'!B:B, MATCH(A23, 'Yards per Pass Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="N23">
+        <f>INDEX('Passing Play % (2023)'!B:B, MATCH(A23, 'Passing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="O23">
+        <f>INDEX('Passing Play % (2013)'!B:B, MATCH(A23, 'Passing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="P23">
+        <f>INDEX('Passing Play % (2003)'!B:B, MATCH(A23, 'Passing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="Q23">
+        <f>INDEX('Win % (2023)'!B:B, MATCH(A23, 'Win % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="R23">
+        <f>INDEX('Win % (2013)'!B:B, MATCH(A23, 'Win % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="S23">
+        <f>INDEX('Win % (2003)'!B:B, MATCH(A23, 'Win % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="T23">
+        <f>INDEX('Completion % (2023)'!B:B, MATCH(A23, 'Completion % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="U23">
+        <f>INDEX('Completion % (2013)'!B:B, MATCH(A23, 'Completion % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="V23">
+        <f>INDEX('Completion % (2003)'!B:B, MATCH(A23, 'Completion % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="W23">
+        <f>INDEX('merged_data_python'!B:B, MATCH(A23, 'merged_data_python'!A:A, 0))</f>
+        <v/>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -11100,6 +13036,94 @@
           <t>Jacksonville</t>
         </is>
       </c>
+      <c r="B24">
+        <f>INDEX('Points Per Game'!B:B, MATCH(A24, 'Points Per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="C24">
+        <f>INDEX('Rushing Attempts per Game'!B:B, MATCH(A24, 'Rushing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="D24">
+        <f>INDEX('Rushing Yards per Game'!B:B, MATCH(A24, 'Rushing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="E24">
+        <f>INDEX('Rushing Touchdowns %'!B:B, MATCH(A24, 'Rushing Touchdowns %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="F24">
+        <f>INDEX('Yards per Rush Attempt'!B:B, MATCH(A24, 'Yards per Rush Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="G24">
+        <f>INDEX('Rushing Play % (2023)'!B:B, MATCH(A24, 'Rushing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="H24">
+        <f>INDEX('Rushing Play % (2013)'!B:B, MATCH(A24, 'Rushing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="I24">
+        <f>INDEX('Rushing Play % (2003)'!B:B, MATCH(A24, 'Rushing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="J24">
+        <f>INDEX('Passing Attempts per Game'!B:B, MATCH(A24, 'Passing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="K24">
+        <f>INDEX('Passing Yards per Game'!B:B, MATCH(A24, 'Passing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="L24">
+        <f>INDEX('Passing Touchdown %'!B:B, MATCH(A24, 'Passing Touchdown %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="M24">
+        <f>INDEX('Yards per Pass Attempt'!B:B, MATCH(A24, 'Yards per Pass Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="N24">
+        <f>INDEX('Passing Play % (2023)'!B:B, MATCH(A24, 'Passing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="O24">
+        <f>INDEX('Passing Play % (2013)'!B:B, MATCH(A24, 'Passing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="P24">
+        <f>INDEX('Passing Play % (2003)'!B:B, MATCH(A24, 'Passing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="Q24">
+        <f>INDEX('Win % (2023)'!B:B, MATCH(A24, 'Win % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="R24">
+        <f>INDEX('Win % (2013)'!B:B, MATCH(A24, 'Win % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="S24">
+        <f>INDEX('Win % (2003)'!B:B, MATCH(A24, 'Win % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="T24">
+        <f>INDEX('Completion % (2023)'!B:B, MATCH(A24, 'Completion % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="U24">
+        <f>INDEX('Completion % (2013)'!B:B, MATCH(A24, 'Completion % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="V24">
+        <f>INDEX('Completion % (2003)'!B:B, MATCH(A24, 'Completion % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="W24">
+        <f>INDEX('merged_data_python'!B:B, MATCH(A24, 'merged_data_python'!A:A, 0))</f>
+        <v/>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -11107,6 +13131,94 @@
           <t>NY Jets</t>
         </is>
       </c>
+      <c r="B25">
+        <f>INDEX('Points Per Game'!B:B, MATCH(A25, 'Points Per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="C25">
+        <f>INDEX('Rushing Attempts per Game'!B:B, MATCH(A25, 'Rushing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="D25">
+        <f>INDEX('Rushing Yards per Game'!B:B, MATCH(A25, 'Rushing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="E25">
+        <f>INDEX('Rushing Touchdowns %'!B:B, MATCH(A25, 'Rushing Touchdowns %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="F25">
+        <f>INDEX('Yards per Rush Attempt'!B:B, MATCH(A25, 'Yards per Rush Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="G25">
+        <f>INDEX('Rushing Play % (2023)'!B:B, MATCH(A25, 'Rushing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="H25">
+        <f>INDEX('Rushing Play % (2013)'!B:B, MATCH(A25, 'Rushing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="I25">
+        <f>INDEX('Rushing Play % (2003)'!B:B, MATCH(A25, 'Rushing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="J25">
+        <f>INDEX('Passing Attempts per Game'!B:B, MATCH(A25, 'Passing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="K25">
+        <f>INDEX('Passing Yards per Game'!B:B, MATCH(A25, 'Passing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="L25">
+        <f>INDEX('Passing Touchdown %'!B:B, MATCH(A25, 'Passing Touchdown %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="M25">
+        <f>INDEX('Yards per Pass Attempt'!B:B, MATCH(A25, 'Yards per Pass Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="N25">
+        <f>INDEX('Passing Play % (2023)'!B:B, MATCH(A25, 'Passing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="O25">
+        <f>INDEX('Passing Play % (2013)'!B:B, MATCH(A25, 'Passing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="P25">
+        <f>INDEX('Passing Play % (2003)'!B:B, MATCH(A25, 'Passing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="Q25">
+        <f>INDEX('Win % (2023)'!B:B, MATCH(A25, 'Win % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="R25">
+        <f>INDEX('Win % (2013)'!B:B, MATCH(A25, 'Win % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="S25">
+        <f>INDEX('Win % (2003)'!B:B, MATCH(A25, 'Win % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="T25">
+        <f>INDEX('Completion % (2023)'!B:B, MATCH(A25, 'Completion % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="U25">
+        <f>INDEX('Completion % (2013)'!B:B, MATCH(A25, 'Completion % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="V25">
+        <f>INDEX('Completion % (2003)'!B:B, MATCH(A25, 'Completion % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="W25">
+        <f>INDEX('merged_data_python'!B:B, MATCH(A25, 'merged_data_python'!A:A, 0))</f>
+        <v/>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -11114,6 +13226,94 @@
           <t>LA Rams</t>
         </is>
       </c>
+      <c r="B26">
+        <f>INDEX('Points Per Game'!B:B, MATCH(A26, 'Points Per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="C26">
+        <f>INDEX('Rushing Attempts per Game'!B:B, MATCH(A26, 'Rushing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="D26">
+        <f>INDEX('Rushing Yards per Game'!B:B, MATCH(A26, 'Rushing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="E26">
+        <f>INDEX('Rushing Touchdowns %'!B:B, MATCH(A26, 'Rushing Touchdowns %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="F26">
+        <f>INDEX('Yards per Rush Attempt'!B:B, MATCH(A26, 'Yards per Rush Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="G26">
+        <f>INDEX('Rushing Play % (2023)'!B:B, MATCH(A26, 'Rushing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="H26">
+        <f>INDEX('Rushing Play % (2013)'!B:B, MATCH(A26, 'Rushing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="I26">
+        <f>INDEX('Rushing Play % (2003)'!B:B, MATCH(A26, 'Rushing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="J26">
+        <f>INDEX('Passing Attempts per Game'!B:B, MATCH(A26, 'Passing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="K26">
+        <f>INDEX('Passing Yards per Game'!B:B, MATCH(A26, 'Passing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="L26">
+        <f>INDEX('Passing Touchdown %'!B:B, MATCH(A26, 'Passing Touchdown %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="M26">
+        <f>INDEX('Yards per Pass Attempt'!B:B, MATCH(A26, 'Yards per Pass Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="N26">
+        <f>INDEX('Passing Play % (2023)'!B:B, MATCH(A26, 'Passing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="O26">
+        <f>INDEX('Passing Play % (2013)'!B:B, MATCH(A26, 'Passing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="P26">
+        <f>INDEX('Passing Play % (2003)'!B:B, MATCH(A26, 'Passing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="Q26">
+        <f>INDEX('Win % (2023)'!B:B, MATCH(A26, 'Win % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="R26">
+        <f>INDEX('Win % (2013)'!B:B, MATCH(A26, 'Win % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="S26">
+        <f>INDEX('Win % (2003)'!B:B, MATCH(A26, 'Win % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="T26">
+        <f>INDEX('Completion % (2023)'!B:B, MATCH(A26, 'Completion % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="U26">
+        <f>INDEX('Completion % (2013)'!B:B, MATCH(A26, 'Completion % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="V26">
+        <f>INDEX('Completion % (2003)'!B:B, MATCH(A26, 'Completion % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="W26">
+        <f>INDEX('merged_data_python'!B:B, MATCH(A26, 'merged_data_python'!A:A, 0))</f>
+        <v/>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -11121,6 +13321,94 @@
           <t>LA Chargers</t>
         </is>
       </c>
+      <c r="B27">
+        <f>INDEX('Points Per Game'!B:B, MATCH(A27, 'Points Per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="C27">
+        <f>INDEX('Rushing Attempts per Game'!B:B, MATCH(A27, 'Rushing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="D27">
+        <f>INDEX('Rushing Yards per Game'!B:B, MATCH(A27, 'Rushing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="E27">
+        <f>INDEX('Rushing Touchdowns %'!B:B, MATCH(A27, 'Rushing Touchdowns %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="F27">
+        <f>INDEX('Yards per Rush Attempt'!B:B, MATCH(A27, 'Yards per Rush Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="G27">
+        <f>INDEX('Rushing Play % (2023)'!B:B, MATCH(A27, 'Rushing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="H27">
+        <f>INDEX('Rushing Play % (2013)'!B:B, MATCH(A27, 'Rushing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="I27">
+        <f>INDEX('Rushing Play % (2003)'!B:B, MATCH(A27, 'Rushing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="J27">
+        <f>INDEX('Passing Attempts per Game'!B:B, MATCH(A27, 'Passing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="K27">
+        <f>INDEX('Passing Yards per Game'!B:B, MATCH(A27, 'Passing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="L27">
+        <f>INDEX('Passing Touchdown %'!B:B, MATCH(A27, 'Passing Touchdown %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="M27">
+        <f>INDEX('Yards per Pass Attempt'!B:B, MATCH(A27, 'Yards per Pass Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="N27">
+        <f>INDEX('Passing Play % (2023)'!B:B, MATCH(A27, 'Passing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="O27">
+        <f>INDEX('Passing Play % (2013)'!B:B, MATCH(A27, 'Passing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="P27">
+        <f>INDEX('Passing Play % (2003)'!B:B, MATCH(A27, 'Passing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="Q27">
+        <f>INDEX('Win % (2023)'!B:B, MATCH(A27, 'Win % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="R27">
+        <f>INDEX('Win % (2013)'!B:B, MATCH(A27, 'Win % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="S27">
+        <f>INDEX('Win % (2003)'!B:B, MATCH(A27, 'Win % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="T27">
+        <f>INDEX('Completion % (2023)'!B:B, MATCH(A27, 'Completion % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="U27">
+        <f>INDEX('Completion % (2013)'!B:B, MATCH(A27, 'Completion % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="V27">
+        <f>INDEX('Completion % (2003)'!B:B, MATCH(A27, 'Completion % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="W27">
+        <f>INDEX('merged_data_python'!B:B, MATCH(A27, 'merged_data_python'!A:A, 0))</f>
+        <v/>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -11128,6 +13416,94 @@
           <t>Las Vegas</t>
         </is>
       </c>
+      <c r="B28">
+        <f>INDEX('Points Per Game'!B:B, MATCH(A28, 'Points Per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="C28">
+        <f>INDEX('Rushing Attempts per Game'!B:B, MATCH(A28, 'Rushing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="D28">
+        <f>INDEX('Rushing Yards per Game'!B:B, MATCH(A28, 'Rushing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="E28">
+        <f>INDEX('Rushing Touchdowns %'!B:B, MATCH(A28, 'Rushing Touchdowns %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="F28">
+        <f>INDEX('Yards per Rush Attempt'!B:B, MATCH(A28, 'Yards per Rush Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="G28">
+        <f>INDEX('Rushing Play % (2023)'!B:B, MATCH(A28, 'Rushing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="H28">
+        <f>INDEX('Rushing Play % (2013)'!B:B, MATCH(A28, 'Rushing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="I28">
+        <f>INDEX('Rushing Play % (2003)'!B:B, MATCH(A28, 'Rushing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="J28">
+        <f>INDEX('Passing Attempts per Game'!B:B, MATCH(A28, 'Passing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="K28">
+        <f>INDEX('Passing Yards per Game'!B:B, MATCH(A28, 'Passing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="L28">
+        <f>INDEX('Passing Touchdown %'!B:B, MATCH(A28, 'Passing Touchdown %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="M28">
+        <f>INDEX('Yards per Pass Attempt'!B:B, MATCH(A28, 'Yards per Pass Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="N28">
+        <f>INDEX('Passing Play % (2023)'!B:B, MATCH(A28, 'Passing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="O28">
+        <f>INDEX('Passing Play % (2013)'!B:B, MATCH(A28, 'Passing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="P28">
+        <f>INDEX('Passing Play % (2003)'!B:B, MATCH(A28, 'Passing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="Q28">
+        <f>INDEX('Win % (2023)'!B:B, MATCH(A28, 'Win % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="R28">
+        <f>INDEX('Win % (2013)'!B:B, MATCH(A28, 'Win % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="S28">
+        <f>INDEX('Win % (2003)'!B:B, MATCH(A28, 'Win % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="T28">
+        <f>INDEX('Completion % (2023)'!B:B, MATCH(A28, 'Completion % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="U28">
+        <f>INDEX('Completion % (2013)'!B:B, MATCH(A28, 'Completion % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="V28">
+        <f>INDEX('Completion % (2003)'!B:B, MATCH(A28, 'Completion % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="W28">
+        <f>INDEX('merged_data_python'!B:B, MATCH(A28, 'merged_data_python'!A:A, 0))</f>
+        <v/>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -11135,6 +13511,94 @@
           <t>Carolina</t>
         </is>
       </c>
+      <c r="B29">
+        <f>INDEX('Points Per Game'!B:B, MATCH(A29, 'Points Per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="C29">
+        <f>INDEX('Rushing Attempts per Game'!B:B, MATCH(A29, 'Rushing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="D29">
+        <f>INDEX('Rushing Yards per Game'!B:B, MATCH(A29, 'Rushing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="E29">
+        <f>INDEX('Rushing Touchdowns %'!B:B, MATCH(A29, 'Rushing Touchdowns %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="F29">
+        <f>INDEX('Yards per Rush Attempt'!B:B, MATCH(A29, 'Yards per Rush Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="G29">
+        <f>INDEX('Rushing Play % (2023)'!B:B, MATCH(A29, 'Rushing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="H29">
+        <f>INDEX('Rushing Play % (2013)'!B:B, MATCH(A29, 'Rushing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="I29">
+        <f>INDEX('Rushing Play % (2003)'!B:B, MATCH(A29, 'Rushing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="J29">
+        <f>INDEX('Passing Attempts per Game'!B:B, MATCH(A29, 'Passing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="K29">
+        <f>INDEX('Passing Yards per Game'!B:B, MATCH(A29, 'Passing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="L29">
+        <f>INDEX('Passing Touchdown %'!B:B, MATCH(A29, 'Passing Touchdown %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="M29">
+        <f>INDEX('Yards per Pass Attempt'!B:B, MATCH(A29, 'Yards per Pass Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="N29">
+        <f>INDEX('Passing Play % (2023)'!B:B, MATCH(A29, 'Passing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="O29">
+        <f>INDEX('Passing Play % (2013)'!B:B, MATCH(A29, 'Passing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="P29">
+        <f>INDEX('Passing Play % (2003)'!B:B, MATCH(A29, 'Passing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="Q29">
+        <f>INDEX('Win % (2023)'!B:B, MATCH(A29, 'Win % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="R29">
+        <f>INDEX('Win % (2013)'!B:B, MATCH(A29, 'Win % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="S29">
+        <f>INDEX('Win % (2003)'!B:B, MATCH(A29, 'Win % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="T29">
+        <f>INDEX('Completion % (2023)'!B:B, MATCH(A29, 'Completion % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="U29">
+        <f>INDEX('Completion % (2013)'!B:B, MATCH(A29, 'Completion % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="V29">
+        <f>INDEX('Completion % (2003)'!B:B, MATCH(A29, 'Completion % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="W29">
+        <f>INDEX('merged_data_python'!B:B, MATCH(A29, 'merged_data_python'!A:A, 0))</f>
+        <v/>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -11142,6 +13606,94 @@
           <t>NY Giants</t>
         </is>
       </c>
+      <c r="B30">
+        <f>INDEX('Points Per Game'!B:B, MATCH(A30, 'Points Per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="C30">
+        <f>INDEX('Rushing Attempts per Game'!B:B, MATCH(A30, 'Rushing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="D30">
+        <f>INDEX('Rushing Yards per Game'!B:B, MATCH(A30, 'Rushing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="E30">
+        <f>INDEX('Rushing Touchdowns %'!B:B, MATCH(A30, 'Rushing Touchdowns %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="F30">
+        <f>INDEX('Yards per Rush Attempt'!B:B, MATCH(A30, 'Yards per Rush Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="G30">
+        <f>INDEX('Rushing Play % (2023)'!B:B, MATCH(A30, 'Rushing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="H30">
+        <f>INDEX('Rushing Play % (2013)'!B:B, MATCH(A30, 'Rushing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="I30">
+        <f>INDEX('Rushing Play % (2003)'!B:B, MATCH(A30, 'Rushing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="J30">
+        <f>INDEX('Passing Attempts per Game'!B:B, MATCH(A30, 'Passing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="K30">
+        <f>INDEX('Passing Yards per Game'!B:B, MATCH(A30, 'Passing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="L30">
+        <f>INDEX('Passing Touchdown %'!B:B, MATCH(A30, 'Passing Touchdown %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="M30">
+        <f>INDEX('Yards per Pass Attempt'!B:B, MATCH(A30, 'Yards per Pass Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="N30">
+        <f>INDEX('Passing Play % (2023)'!B:B, MATCH(A30, 'Passing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="O30">
+        <f>INDEX('Passing Play % (2013)'!B:B, MATCH(A30, 'Passing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="P30">
+        <f>INDEX('Passing Play % (2003)'!B:B, MATCH(A30, 'Passing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="Q30">
+        <f>INDEX('Win % (2023)'!B:B, MATCH(A30, 'Win % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="R30">
+        <f>INDEX('Win % (2013)'!B:B, MATCH(A30, 'Win % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="S30">
+        <f>INDEX('Win % (2003)'!B:B, MATCH(A30, 'Win % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="T30">
+        <f>INDEX('Completion % (2023)'!B:B, MATCH(A30, 'Completion % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="U30">
+        <f>INDEX('Completion % (2013)'!B:B, MATCH(A30, 'Completion % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="V30">
+        <f>INDEX('Completion % (2003)'!B:B, MATCH(A30, 'Completion % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="W30">
+        <f>INDEX('merged_data_python'!B:B, MATCH(A30, 'merged_data_python'!A:A, 0))</f>
+        <v/>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -11149,6 +13701,94 @@
           <t>Cleveland</t>
         </is>
       </c>
+      <c r="B31">
+        <f>INDEX('Points Per Game'!B:B, MATCH(A31, 'Points Per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="C31">
+        <f>INDEX('Rushing Attempts per Game'!B:B, MATCH(A31, 'Rushing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="D31">
+        <f>INDEX('Rushing Yards per Game'!B:B, MATCH(A31, 'Rushing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="E31">
+        <f>INDEX('Rushing Touchdowns %'!B:B, MATCH(A31, 'Rushing Touchdowns %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="F31">
+        <f>INDEX('Yards per Rush Attempt'!B:B, MATCH(A31, 'Yards per Rush Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="G31">
+        <f>INDEX('Rushing Play % (2023)'!B:B, MATCH(A31, 'Rushing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="H31">
+        <f>INDEX('Rushing Play % (2013)'!B:B, MATCH(A31, 'Rushing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="I31">
+        <f>INDEX('Rushing Play % (2003)'!B:B, MATCH(A31, 'Rushing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="J31">
+        <f>INDEX('Passing Attempts per Game'!B:B, MATCH(A31, 'Passing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="K31">
+        <f>INDEX('Passing Yards per Game'!B:B, MATCH(A31, 'Passing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="L31">
+        <f>INDEX('Passing Touchdown %'!B:B, MATCH(A31, 'Passing Touchdown %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="M31">
+        <f>INDEX('Yards per Pass Attempt'!B:B, MATCH(A31, 'Yards per Pass Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="N31">
+        <f>INDEX('Passing Play % (2023)'!B:B, MATCH(A31, 'Passing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="O31">
+        <f>INDEX('Passing Play % (2013)'!B:B, MATCH(A31, 'Passing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="P31">
+        <f>INDEX('Passing Play % (2003)'!B:B, MATCH(A31, 'Passing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="Q31">
+        <f>INDEX('Win % (2023)'!B:B, MATCH(A31, 'Win % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="R31">
+        <f>INDEX('Win % (2013)'!B:B, MATCH(A31, 'Win % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="S31">
+        <f>INDEX('Win % (2003)'!B:B, MATCH(A31, 'Win % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="T31">
+        <f>INDEX('Completion % (2023)'!B:B, MATCH(A31, 'Completion % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="U31">
+        <f>INDEX('Completion % (2013)'!B:B, MATCH(A31, 'Completion % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="V31">
+        <f>INDEX('Completion % (2003)'!B:B, MATCH(A31, 'Completion % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="W31">
+        <f>INDEX('merged_data_python'!B:B, MATCH(A31, 'merged_data_python'!A:A, 0))</f>
+        <v/>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -11156,12 +13796,188 @@
           <t>New England</t>
         </is>
       </c>
+      <c r="B32">
+        <f>INDEX('Points Per Game'!B:B, MATCH(A32, 'Points Per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="C32">
+        <f>INDEX('Rushing Attempts per Game'!B:B, MATCH(A32, 'Rushing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="D32">
+        <f>INDEX('Rushing Yards per Game'!B:B, MATCH(A32, 'Rushing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="E32">
+        <f>INDEX('Rushing Touchdowns %'!B:B, MATCH(A32, 'Rushing Touchdowns %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="F32">
+        <f>INDEX('Yards per Rush Attempt'!B:B, MATCH(A32, 'Yards per Rush Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="G32">
+        <f>INDEX('Rushing Play % (2023)'!B:B, MATCH(A32, 'Rushing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="H32">
+        <f>INDEX('Rushing Play % (2013)'!B:B, MATCH(A32, 'Rushing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="I32">
+        <f>INDEX('Rushing Play % (2003)'!B:B, MATCH(A32, 'Rushing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="J32">
+        <f>INDEX('Passing Attempts per Game'!B:B, MATCH(A32, 'Passing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="K32">
+        <f>INDEX('Passing Yards per Game'!B:B, MATCH(A32, 'Passing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="L32">
+        <f>INDEX('Passing Touchdown %'!B:B, MATCH(A32, 'Passing Touchdown %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="M32">
+        <f>INDEX('Yards per Pass Attempt'!B:B, MATCH(A32, 'Yards per Pass Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="N32">
+        <f>INDEX('Passing Play % (2023)'!B:B, MATCH(A32, 'Passing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="O32">
+        <f>INDEX('Passing Play % (2013)'!B:B, MATCH(A32, 'Passing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="P32">
+        <f>INDEX('Passing Play % (2003)'!B:B, MATCH(A32, 'Passing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="Q32">
+        <f>INDEX('Win % (2023)'!B:B, MATCH(A32, 'Win % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="R32">
+        <f>INDEX('Win % (2013)'!B:B, MATCH(A32, 'Win % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="S32">
+        <f>INDEX('Win % (2003)'!B:B, MATCH(A32, 'Win % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="T32">
+        <f>INDEX('Completion % (2023)'!B:B, MATCH(A32, 'Completion % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="U32">
+        <f>INDEX('Completion % (2013)'!B:B, MATCH(A32, 'Completion % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="V32">
+        <f>INDEX('Completion % (2003)'!B:B, MATCH(A32, 'Completion % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="W32">
+        <f>INDEX('merged_data_python'!B:B, MATCH(A32, 'merged_data_python'!A:A, 0))</f>
+        <v/>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
           <t>Miami</t>
         </is>
+      </c>
+      <c r="B33">
+        <f>INDEX('Points Per Game'!B:B, MATCH(A33, 'Points Per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="C33">
+        <f>INDEX('Rushing Attempts per Game'!B:B, MATCH(A33, 'Rushing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="D33">
+        <f>INDEX('Rushing Yards per Game'!B:B, MATCH(A33, 'Rushing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="E33">
+        <f>INDEX('Rushing Touchdowns %'!B:B, MATCH(A33, 'Rushing Touchdowns %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="F33">
+        <f>INDEX('Yards per Rush Attempt'!B:B, MATCH(A33, 'Yards per Rush Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="G33">
+        <f>INDEX('Rushing Play % (2023)'!B:B, MATCH(A33, 'Rushing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="H33">
+        <f>INDEX('Rushing Play % (2013)'!B:B, MATCH(A33, 'Rushing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="I33">
+        <f>INDEX('Rushing Play % (2003)'!B:B, MATCH(A33, 'Rushing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="J33">
+        <f>INDEX('Passing Attempts per Game'!B:B, MATCH(A33, 'Passing Attempts per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="K33">
+        <f>INDEX('Passing Yards per Game'!B:B, MATCH(A33, 'Passing Yards per Game'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="L33">
+        <f>INDEX('Passing Touchdown %'!B:B, MATCH(A33, 'Passing Touchdown %'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="M33">
+        <f>INDEX('Yards per Pass Attempt'!B:B, MATCH(A33, 'Yards per Pass Attempt'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="N33">
+        <f>INDEX('Passing Play % (2023)'!B:B, MATCH(A33, 'Passing Play % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="O33">
+        <f>INDEX('Passing Play % (2013)'!B:B, MATCH(A33, 'Passing Play % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="P33">
+        <f>INDEX('Passing Play % (2003)'!B:B, MATCH(A33, 'Passing Play % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="Q33">
+        <f>INDEX('Win % (2023)'!B:B, MATCH(A33, 'Win % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="R33">
+        <f>INDEX('Win % (2013)'!B:B, MATCH(A33, 'Win % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="S33">
+        <f>INDEX('Win % (2003)'!B:B, MATCH(A33, 'Win % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="T33">
+        <f>INDEX('Completion % (2023)'!B:B, MATCH(A33, 'Completion % (2023)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="U33">
+        <f>INDEX('Completion % (2013)'!B:B, MATCH(A33, 'Completion % (2013)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="V33">
+        <f>INDEX('Completion % (2003)'!B:B, MATCH(A33, 'Completion % (2003)'!A:A, 0))</f>
+        <v/>
+      </c>
+      <c r="W33">
+        <f>INDEX('merged_data_python'!B:B, MATCH(A33, 'merged_data_python'!A:A, 0))</f>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -11181,7 +13997,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13.5" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
@@ -12825,7 +15641,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13.33203125" customWidth="1" min="1" max="1"/>
   </cols>

</xml_diff>

<commit_message>
added wrtie headers to sheet function
</commit_message>
<xml_diff>
--- a/transformation_workbook.xlsx
+++ b/transformation_workbook.xlsx
@@ -10820,7 +10820,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V33"/>
+  <dimension ref="A1:A33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10832,111 +10832,6 @@
       <c r="A1" t="inlineStr">
         <is>
           <t>Team</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Points Per Game</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Rushing Attempts per Game</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Rushing Yards per Game</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Rushing Touchdowns %</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Yards per Rush Attempt</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Rushing Play % (2023)</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Rushing Play % (2013)</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Rushing Play % (2003)</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>Passing Attempts per Game</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>Passing Yards per Game</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>Passing Touchdown %</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>Yards per Pass Attempt</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>Passing Play % (2023)</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>Passing Play % (2013)</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>Passing Play % (2003)</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>Win % (2023)</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>Win % (2013)</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>Win % (2003)</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>Completion % (2023)</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>Completion % (2013)</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>Completion % (2003)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed spelling in file path
</commit_message>
<xml_diff>
--- a/transformation_workbook.xlsx
+++ b/transformation_workbook.xlsx
@@ -10820,7 +10820,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A33"/>
+  <dimension ref="A1:V33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10832,6 +10832,111 @@
       <c r="A1" t="inlineStr">
         <is>
           <t>Team</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Points Per Game</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Rushing Attempts per Game</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Rushing Yards per Game</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Rushing Touchdowns %</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Yards per Rush Attempt</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Rushing Play % (2023)</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Rushing Play % (2013)</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Rushing Play % (2003)</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Passing Attempts per Game</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Passing Yards per Game</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Passing Touchdown %</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Yards per Pass Attempt</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Passing Play % (2023)</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Passing Play % (2013)</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>Passing Play % (2003)</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>Win % (2023)</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>Win % (2013)</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>Win % (2003)</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>Completion % (2023)</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>Completion % (2013)</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>Completion % (2003)</t>
         </is>
       </c>
     </row>

</xml_diff>